<commit_message>
Added the GPS points of the sites in .xlsx files to ease the mapping.
</commit_message>
<xml_diff>
--- a/data/field_data/field_data_summer_2017_pcr.xlsx
+++ b/data/field_data/field_data_summer_2017_pcr.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10812"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11108"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JeremieBoudreault/Google Drive/Coding Projects/HSC_curves_FDA/Habitat_suitability_curves_functional_data_analysis/data/field data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JeremieBoudreault/Google Drive/Coding Projects/2_in_progress/habitat_suitability_curves_fda/data/field_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A96FB66-4050-7E40-9927-36BEFB28C85D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93CEF20D-DFC5-944C-BFA5-64B615FC3BCC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14140" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14140" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mesures" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,10 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -39,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="148">
   <si>
     <t>Site</t>
   </si>
@@ -771,7 +774,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="101">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -992,21 +995,6 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1035,6 +1023,24 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1319,11 +1325,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CO1049"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="87" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane xSplit="5" ySplit="3" topLeftCell="N698" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="87" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+      <pane xSplit="5" ySplit="3" topLeftCell="AD18" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="E18" sqref="E18:E1049"/>
+      <selection pane="bottomRight" activeCell="AI699" sqref="AI219:AI699"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1360,48 +1366,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:93" s="61" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A1" s="89" t="s">
+      <c r="A1" s="99" t="s">
         <v>95</v>
       </c>
-      <c r="B1" s="89"/>
-      <c r="C1" s="89"/>
-      <c r="D1" s="89"/>
-      <c r="E1" s="90"/>
-      <c r="F1" s="86" t="s">
+      <c r="B1" s="99"/>
+      <c r="C1" s="99"/>
+      <c r="D1" s="99"/>
+      <c r="E1" s="100"/>
+      <c r="F1" s="96" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="87"/>
-      <c r="H1" s="87"/>
-      <c r="I1" s="87"/>
-      <c r="J1" s="87"/>
-      <c r="K1" s="87"/>
-      <c r="L1" s="87"/>
-      <c r="M1" s="87"/>
-      <c r="N1" s="88"/>
-      <c r="O1" s="86" t="s">
+      <c r="G1" s="97"/>
+      <c r="H1" s="97"/>
+      <c r="I1" s="97"/>
+      <c r="J1" s="97"/>
+      <c r="K1" s="97"/>
+      <c r="L1" s="97"/>
+      <c r="M1" s="97"/>
+      <c r="N1" s="98"/>
+      <c r="O1" s="96" t="s">
         <v>19</v>
       </c>
-      <c r="P1" s="87"/>
-      <c r="Q1" s="87"/>
-      <c r="R1" s="87"/>
-      <c r="S1" s="87"/>
-      <c r="T1" s="87"/>
-      <c r="U1" s="87"/>
-      <c r="V1" s="87"/>
-      <c r="W1" s="88"/>
-      <c r="X1" s="86" t="s">
+      <c r="P1" s="97"/>
+      <c r="Q1" s="97"/>
+      <c r="R1" s="97"/>
+      <c r="S1" s="97"/>
+      <c r="T1" s="97"/>
+      <c r="U1" s="97"/>
+      <c r="V1" s="97"/>
+      <c r="W1" s="98"/>
+      <c r="X1" s="96" t="s">
         <v>29</v>
       </c>
-      <c r="Y1" s="87"/>
-      <c r="Z1" s="87"/>
-      <c r="AA1" s="87"/>
-      <c r="AB1" s="87"/>
-      <c r="AC1" s="87"/>
-      <c r="AD1" s="87"/>
-      <c r="AE1" s="87"/>
-      <c r="AF1" s="87"/>
-      <c r="AG1" s="87"/>
-      <c r="AH1" s="88"/>
+      <c r="Y1" s="97"/>
+      <c r="Z1" s="97"/>
+      <c r="AA1" s="97"/>
+      <c r="AB1" s="97"/>
+      <c r="AC1" s="97"/>
+      <c r="AD1" s="97"/>
+      <c r="AE1" s="97"/>
+      <c r="AF1" s="97"/>
+      <c r="AG1" s="97"/>
+      <c r="AH1" s="98"/>
     </row>
     <row r="2" spans="1:93" s="16" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="36" t="s">
@@ -2684,7 +2690,7 @@
       <c r="C18" s="3">
         <v>15</v>
       </c>
-      <c r="E18" s="92"/>
+      <c r="E18" s="87"/>
       <c r="F18" s="44">
         <v>0.36199999999999999</v>
       </c>
@@ -2740,7 +2746,7 @@
       <c r="C19" s="3">
         <v>16</v>
       </c>
-      <c r="E19" s="92"/>
+      <c r="E19" s="87"/>
       <c r="F19" s="44">
         <v>0.36499999999999999</v>
       </c>
@@ -2800,7 +2806,7 @@
       <c r="C20" s="3">
         <v>17</v>
       </c>
-      <c r="E20" s="92"/>
+      <c r="E20" s="87"/>
       <c r="F20" s="44">
         <v>0.27700000000000002</v>
       </c>
@@ -2863,7 +2869,7 @@
       <c r="D21" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E21" s="93"/>
+      <c r="E21" s="88"/>
       <c r="F21" s="46">
         <v>0.23799999999999999</v>
       </c>
@@ -2985,7 +2991,7 @@
       <c r="D22" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E22" s="92"/>
+      <c r="E22" s="87"/>
       <c r="F22" s="44">
         <v>0.245</v>
       </c>
@@ -3047,7 +3053,7 @@
       <c r="C23" s="3">
         <v>20</v>
       </c>
-      <c r="E23" s="92"/>
+      <c r="E23" s="87"/>
       <c r="F23" s="44">
         <v>0.23699999999999999</v>
       </c>
@@ -3105,7 +3111,7 @@
       <c r="C24" s="3">
         <v>21</v>
       </c>
-      <c r="E24" s="92"/>
+      <c r="E24" s="87"/>
       <c r="F24" s="44">
         <v>0.183</v>
       </c>
@@ -3161,7 +3167,7 @@
       <c r="C25" s="3">
         <v>22</v>
       </c>
-      <c r="E25" s="92"/>
+      <c r="E25" s="87"/>
       <c r="F25" s="44">
         <v>0.311</v>
       </c>
@@ -3217,7 +3223,7 @@
       <c r="C26" s="3">
         <v>23</v>
       </c>
-      <c r="E26" s="92"/>
+      <c r="E26" s="87"/>
       <c r="F26" s="44">
         <v>0.43099999999999999</v>
       </c>
@@ -3278,7 +3284,7 @@
       <c r="D27" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E27" s="93"/>
+      <c r="E27" s="88"/>
       <c r="F27" s="46">
         <v>0.19</v>
       </c>
@@ -3396,7 +3402,7 @@
       <c r="D28" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E28" s="92"/>
+      <c r="E28" s="87"/>
       <c r="F28" s="44">
         <v>0.43099999999999999</v>
       </c>
@@ -3454,7 +3460,7 @@
       <c r="C29" s="3">
         <v>26</v>
       </c>
-      <c r="E29" s="92"/>
+      <c r="E29" s="87"/>
       <c r="F29" s="44">
         <v>0.48899999999999999</v>
       </c>
@@ -3510,7 +3516,7 @@
       <c r="C30" s="3">
         <v>27</v>
       </c>
-      <c r="E30" s="92"/>
+      <c r="E30" s="87"/>
       <c r="F30" s="44">
         <v>0.441</v>
       </c>
@@ -3568,7 +3574,7 @@
       <c r="C31" s="3">
         <v>28</v>
       </c>
-      <c r="E31" s="92"/>
+      <c r="E31" s="87"/>
       <c r="F31" s="44">
         <v>0.20200000000000001</v>
       </c>
@@ -3624,7 +3630,7 @@
       <c r="C32" s="3">
         <v>29</v>
       </c>
-      <c r="E32" s="92"/>
+      <c r="E32" s="87"/>
       <c r="F32" s="44">
         <v>6.0999999999999999E-2</v>
       </c>
@@ -3689,7 +3695,7 @@
       <c r="D33" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="E33" s="94"/>
+      <c r="E33" s="89"/>
       <c r="F33" s="48">
         <v>0.27100000000000002</v>
       </c>
@@ -3809,7 +3815,7 @@
       <c r="D34" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="E34" s="92">
+      <c r="E34" s="87">
         <v>1364</v>
       </c>
       <c r="F34" s="44">
@@ -3872,7 +3878,7 @@
         <v>2</v>
       </c>
       <c r="D35" s="38"/>
-      <c r="E35" s="92">
+      <c r="E35" s="87">
         <v>1365</v>
       </c>
       <c r="F35" s="44">
@@ -3931,7 +3937,7 @@
       <c r="D36" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="E36" s="92">
+      <c r="E36" s="87">
         <v>1366</v>
       </c>
       <c r="F36" s="44">
@@ -3994,7 +4000,7 @@
       <c r="D37" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="E37" s="92">
+      <c r="E37" s="87">
         <v>1367</v>
       </c>
       <c r="F37" s="44">
@@ -4055,7 +4061,7 @@
         <v>5</v>
       </c>
       <c r="D38" s="38"/>
-      <c r="E38" s="92">
+      <c r="E38" s="87">
         <v>1368</v>
       </c>
       <c r="F38" s="44">
@@ -4114,7 +4120,7 @@
       <c r="D39" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="E39" s="93">
+      <c r="E39" s="88">
         <v>1369</v>
       </c>
       <c r="F39" s="46">
@@ -4236,7 +4242,7 @@
       <c r="D40" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="E40" s="92">
+      <c r="E40" s="87">
         <v>1370</v>
       </c>
       <c r="F40" s="44">
@@ -4297,7 +4303,7 @@
         <v>8</v>
       </c>
       <c r="D41" s="38"/>
-      <c r="E41" s="92">
+      <c r="E41" s="87">
         <v>1371</v>
       </c>
       <c r="F41" s="44">
@@ -4358,7 +4364,7 @@
         <v>9</v>
       </c>
       <c r="D42" s="38"/>
-      <c r="E42" s="92">
+      <c r="E42" s="87">
         <v>1372</v>
       </c>
       <c r="F42" s="44">
@@ -4417,7 +4423,7 @@
         <v>10</v>
       </c>
       <c r="D43" s="38"/>
-      <c r="E43" s="92">
+      <c r="E43" s="87">
         <v>1373</v>
       </c>
       <c r="F43" s="44">
@@ -4478,7 +4484,7 @@
         <v>11</v>
       </c>
       <c r="D44" s="38"/>
-      <c r="E44" s="92">
+      <c r="E44" s="87">
         <v>1374</v>
       </c>
       <c r="F44" s="44">
@@ -4539,7 +4545,7 @@
       <c r="D45" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="E45" s="93">
+      <c r="E45" s="88">
         <v>1375</v>
       </c>
       <c r="F45" s="46">
@@ -4657,7 +4663,7 @@
       <c r="D46" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="E46" s="92">
+      <c r="E46" s="87">
         <v>1376</v>
       </c>
       <c r="F46" s="44">
@@ -4716,7 +4722,7 @@
         <v>14</v>
       </c>
       <c r="D47" s="38"/>
-      <c r="E47" s="92">
+      <c r="E47" s="87">
         <v>1377</v>
       </c>
       <c r="F47" s="44">
@@ -4775,7 +4781,7 @@
         <v>15</v>
       </c>
       <c r="D48" s="38"/>
-      <c r="E48" s="92">
+      <c r="E48" s="87">
         <v>1378</v>
       </c>
       <c r="F48" s="44">
@@ -4834,7 +4840,7 @@
         <v>16</v>
       </c>
       <c r="D49" s="38"/>
-      <c r="E49" s="92">
+      <c r="E49" s="87">
         <v>1379</v>
       </c>
       <c r="F49" s="44">
@@ -4895,7 +4901,7 @@
         <v>17</v>
       </c>
       <c r="D50" s="38"/>
-      <c r="E50" s="92">
+      <c r="E50" s="87">
         <v>1380</v>
       </c>
       <c r="F50" s="44">
@@ -4954,7 +4960,7 @@
       <c r="D51" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="E51" s="93">
+      <c r="E51" s="88">
         <v>1381</v>
       </c>
       <c r="F51" s="46">
@@ -5072,7 +5078,7 @@
       <c r="D52" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="E52" s="92">
+      <c r="E52" s="87">
         <v>1382</v>
       </c>
       <c r="F52" s="44">
@@ -5135,7 +5141,7 @@
         <v>20</v>
       </c>
       <c r="D53" s="38"/>
-      <c r="E53" s="92">
+      <c r="E53" s="87">
         <v>1383</v>
       </c>
       <c r="F53" s="44">
@@ -5192,7 +5198,7 @@
         <v>21</v>
       </c>
       <c r="D54" s="38"/>
-      <c r="E54" s="92">
+      <c r="E54" s="87">
         <v>1384</v>
       </c>
       <c r="F54" s="44">
@@ -5249,7 +5255,7 @@
         <v>22</v>
       </c>
       <c r="D55" s="38"/>
-      <c r="E55" s="92">
+      <c r="E55" s="87">
         <v>1385</v>
       </c>
       <c r="F55" s="44">
@@ -5310,7 +5316,7 @@
         <v>23</v>
       </c>
       <c r="D56" s="38"/>
-      <c r="E56" s="92">
+      <c r="E56" s="87">
         <v>1386</v>
       </c>
       <c r="F56" s="44">
@@ -5371,7 +5377,7 @@
       <c r="D57" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="E57" s="93">
+      <c r="E57" s="88">
         <v>1387</v>
       </c>
       <c r="F57" s="46">
@@ -5493,7 +5499,7 @@
       <c r="D58" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="E58" s="92">
+      <c r="E58" s="87">
         <v>1388</v>
       </c>
       <c r="F58" s="44">
@@ -5554,7 +5560,7 @@
         <v>26</v>
       </c>
       <c r="D59" s="38"/>
-      <c r="E59" s="92">
+      <c r="E59" s="87">
         <v>1389</v>
       </c>
       <c r="F59" s="44">
@@ -5617,7 +5623,7 @@
         <v>27</v>
       </c>
       <c r="D60" s="38"/>
-      <c r="E60" s="92">
+      <c r="E60" s="87">
         <v>1390</v>
       </c>
       <c r="F60" s="44">
@@ -5676,7 +5682,7 @@
         <v>28</v>
       </c>
       <c r="D61" s="38"/>
-      <c r="E61" s="92">
+      <c r="E61" s="87">
         <v>1391</v>
       </c>
       <c r="F61" s="44">
@@ -5735,7 +5741,7 @@
         <v>29</v>
       </c>
       <c r="D62" s="38"/>
-      <c r="E62" s="92">
+      <c r="E62" s="87">
         <v>1392</v>
       </c>
       <c r="F62" s="44">
@@ -5798,7 +5804,7 @@
       <c r="D63" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="E63" s="94">
+      <c r="E63" s="89">
         <v>1393</v>
       </c>
       <c r="F63" s="48">
@@ -5918,7 +5924,7 @@
       <c r="D64" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="E64" s="92">
+      <c r="E64" s="87">
         <v>1403</v>
       </c>
       <c r="F64" s="44">
@@ -5981,7 +5987,7 @@
         <v>2</v>
       </c>
       <c r="D65" s="38"/>
-      <c r="E65" s="92">
+      <c r="E65" s="87">
         <v>1404</v>
       </c>
       <c r="F65" s="44">
@@ -6042,7 +6048,7 @@
         <v>3</v>
       </c>
       <c r="D66" s="38"/>
-      <c r="E66" s="92">
+      <c r="E66" s="87">
         <v>1405</v>
       </c>
       <c r="F66" s="44">
@@ -6101,7 +6107,7 @@
         <v>4</v>
       </c>
       <c r="D67" s="38"/>
-      <c r="E67" s="92">
+      <c r="E67" s="87">
         <v>1406</v>
       </c>
       <c r="F67" s="44">
@@ -6158,7 +6164,7 @@
         <v>5</v>
       </c>
       <c r="D68" s="38"/>
-      <c r="E68" s="92">
+      <c r="E68" s="87">
         <v>1407</v>
       </c>
       <c r="F68" s="44">
@@ -6217,7 +6223,7 @@
       <c r="D69" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="E69" s="93">
+      <c r="E69" s="88">
         <v>1408</v>
       </c>
       <c r="F69" s="46">
@@ -6345,7 +6351,7 @@
       <c r="D70" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="E70" s="92">
+      <c r="E70" s="87">
         <v>1409</v>
       </c>
       <c r="F70" s="44">
@@ -6410,7 +6416,7 @@
         <v>8</v>
       </c>
       <c r="D71" s="38"/>
-      <c r="E71" s="92">
+      <c r="E71" s="87">
         <v>1410</v>
       </c>
       <c r="F71" s="44">
@@ -6469,7 +6475,7 @@
         <v>9</v>
       </c>
       <c r="D72" s="38"/>
-      <c r="E72" s="92">
+      <c r="E72" s="87">
         <v>1411</v>
       </c>
       <c r="F72" s="44">
@@ -6532,7 +6538,7 @@
         <v>10</v>
       </c>
       <c r="D73" s="38"/>
-      <c r="E73" s="92">
+      <c r="E73" s="87">
         <v>1412</v>
       </c>
       <c r="F73" s="44">
@@ -6589,7 +6595,7 @@
         <v>11</v>
       </c>
       <c r="D74" s="38"/>
-      <c r="E74" s="92">
+      <c r="E74" s="87">
         <v>1413</v>
       </c>
       <c r="F74" s="44">
@@ -6650,7 +6656,7 @@
       <c r="D75" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="E75" s="93">
+      <c r="E75" s="88">
         <v>1414</v>
       </c>
       <c r="F75" s="46">
@@ -6768,7 +6774,7 @@
       <c r="D76" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="E76" s="92">
+      <c r="E76" s="87">
         <v>1415</v>
       </c>
       <c r="F76" s="44">
@@ -6827,7 +6833,7 @@
         <v>14</v>
       </c>
       <c r="D77" s="38"/>
-      <c r="E77" s="92">
+      <c r="E77" s="87">
         <v>1416</v>
       </c>
       <c r="F77" s="44">
@@ -6886,7 +6892,7 @@
         <v>15</v>
       </c>
       <c r="D78" s="38"/>
-      <c r="E78" s="92">
+      <c r="E78" s="87">
         <v>1417</v>
       </c>
       <c r="F78" s="44">
@@ -6947,7 +6953,7 @@
         <v>16</v>
       </c>
       <c r="D79" s="38"/>
-      <c r="E79" s="92">
+      <c r="E79" s="87">
         <v>1418</v>
       </c>
       <c r="F79" s="44">
@@ -7006,7 +7012,7 @@
         <v>17</v>
       </c>
       <c r="D80" s="38"/>
-      <c r="E80" s="92">
+      <c r="E80" s="87">
         <v>1419</v>
       </c>
       <c r="F80" s="44">
@@ -7073,7 +7079,7 @@
       <c r="D81" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="E81" s="93">
+      <c r="E81" s="88">
         <v>1420</v>
       </c>
       <c r="F81" s="59">
@@ -7196,7 +7202,7 @@
       <c r="D82" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="E82" s="92">
+      <c r="E82" s="87">
         <v>1421</v>
       </c>
       <c r="F82" s="44">
@@ -7257,7 +7263,7 @@
         <v>20</v>
       </c>
       <c r="D83" s="38"/>
-      <c r="E83" s="92">
+      <c r="E83" s="87">
         <v>1422</v>
       </c>
       <c r="F83" s="44">
@@ -7320,7 +7326,7 @@
         <v>21</v>
       </c>
       <c r="D84" s="38"/>
-      <c r="E84" s="92">
+      <c r="E84" s="87">
         <v>1423</v>
       </c>
       <c r="F84" s="44">
@@ -7381,7 +7387,7 @@
         <v>22</v>
       </c>
       <c r="D85" s="38"/>
-      <c r="E85" s="92">
+      <c r="E85" s="87">
         <v>1424</v>
       </c>
       <c r="F85" s="44">
@@ -7450,7 +7456,7 @@
         <v>23</v>
       </c>
       <c r="D86" s="38"/>
-      <c r="E86" s="92">
+      <c r="E86" s="87">
         <v>1425</v>
       </c>
       <c r="F86" s="44">
@@ -7509,7 +7515,7 @@
       <c r="D87" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="E87" s="93">
+      <c r="E87" s="88">
         <v>1426</v>
       </c>
       <c r="F87" s="46">
@@ -7627,7 +7633,7 @@
       <c r="D88" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="E88" s="92">
+      <c r="E88" s="87">
         <v>1427</v>
       </c>
       <c r="F88" s="44">
@@ -7690,7 +7696,7 @@
         <v>26</v>
       </c>
       <c r="D89" s="38"/>
-      <c r="E89" s="92">
+      <c r="E89" s="87">
         <v>1428</v>
       </c>
       <c r="F89" s="44">
@@ -7749,7 +7755,7 @@
         <v>27</v>
       </c>
       <c r="D90" s="38"/>
-      <c r="E90" s="92">
+      <c r="E90" s="87">
         <v>1429</v>
       </c>
       <c r="F90" s="44">
@@ -7808,7 +7814,7 @@
         <v>28</v>
       </c>
       <c r="D91" s="38"/>
-      <c r="E91" s="92">
+      <c r="E91" s="87">
         <v>1430</v>
       </c>
       <c r="F91" s="44">
@@ -7875,7 +7881,7 @@
         <v>29</v>
       </c>
       <c r="D92" s="38"/>
-      <c r="E92" s="92">
+      <c r="E92" s="87">
         <v>1431</v>
       </c>
       <c r="F92" s="44">
@@ -7940,7 +7946,7 @@
       <c r="D93" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="E93" s="94">
+      <c r="E93" s="89">
         <v>1432</v>
       </c>
       <c r="F93" s="58">
@@ -8063,7 +8069,7 @@
       <c r="D94" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="E94" s="92">
+      <c r="E94" s="87">
         <v>1435</v>
       </c>
       <c r="F94" s="44">
@@ -8122,7 +8128,7 @@
         <v>2</v>
       </c>
       <c r="D95" s="38"/>
-      <c r="E95" s="92">
+      <c r="E95" s="87">
         <v>1436</v>
       </c>
       <c r="F95" s="44">
@@ -8181,7 +8187,7 @@
         <v>3</v>
       </c>
       <c r="D96" s="38"/>
-      <c r="E96" s="92">
+      <c r="E96" s="87">
         <v>1437</v>
       </c>
       <c r="F96" s="44">
@@ -8242,7 +8248,7 @@
       <c r="D97" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="E97" s="92">
+      <c r="E97" s="87">
         <v>1438</v>
       </c>
       <c r="F97" s="44">
@@ -8307,7 +8313,7 @@
       <c r="D98" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="E98" s="92">
+      <c r="E98" s="87">
         <v>1439</v>
       </c>
       <c r="F98" s="44">
@@ -8370,7 +8376,7 @@
       <c r="D99" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="E99" s="93">
+      <c r="E99" s="88">
         <v>1440</v>
       </c>
       <c r="F99" s="46">
@@ -8486,7 +8492,7 @@
       <c r="D100" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="E100" s="92">
+      <c r="E100" s="87">
         <v>1441</v>
       </c>
       <c r="F100" s="44">
@@ -8545,7 +8551,7 @@
         <v>8</v>
       </c>
       <c r="D101" s="38"/>
-      <c r="E101" s="92">
+      <c r="E101" s="87">
         <v>1442</v>
       </c>
       <c r="F101" s="44">
@@ -8602,7 +8608,7 @@
         <v>9</v>
       </c>
       <c r="D102" s="38"/>
-      <c r="E102" s="92">
+      <c r="E102" s="87">
         <v>1443</v>
       </c>
       <c r="F102" s="44">
@@ -8665,7 +8671,7 @@
         <v>10</v>
       </c>
       <c r="D103" s="38"/>
-      <c r="E103" s="92">
+      <c r="E103" s="87">
         <v>1444</v>
       </c>
       <c r="F103" s="44">
@@ -8726,7 +8732,7 @@
       <c r="D104" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="E104" s="92">
+      <c r="E104" s="87">
         <v>1445</v>
       </c>
       <c r="F104" s="44">
@@ -8791,7 +8797,7 @@
       <c r="D105" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="E105" s="93">
+      <c r="E105" s="88">
         <v>1446</v>
       </c>
       <c r="F105" s="46">
@@ -8909,7 +8915,7 @@
       <c r="D106" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="E106" s="92">
+      <c r="E106" s="87">
         <v>1447</v>
       </c>
       <c r="F106" s="44">
@@ -8968,7 +8974,7 @@
         <v>14</v>
       </c>
       <c r="D107" s="38"/>
-      <c r="E107" s="92">
+      <c r="E107" s="87">
         <v>1448</v>
       </c>
       <c r="F107" s="44">
@@ -9027,7 +9033,7 @@
         <v>15</v>
       </c>
       <c r="D108" s="38"/>
-      <c r="E108" s="92">
+      <c r="E108" s="87">
         <v>1449</v>
       </c>
       <c r="F108" s="44">
@@ -9086,7 +9092,7 @@
         <v>16</v>
       </c>
       <c r="D109" s="38"/>
-      <c r="E109" s="92">
+      <c r="E109" s="87">
         <v>1450</v>
       </c>
       <c r="F109" s="44">
@@ -9145,7 +9151,7 @@
         <v>17</v>
       </c>
       <c r="D110" s="38"/>
-      <c r="E110" s="92">
+      <c r="E110" s="87">
         <v>1451</v>
       </c>
       <c r="F110" s="44">
@@ -9206,7 +9212,7 @@
       <c r="D111" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="E111" s="93">
+      <c r="E111" s="88">
         <v>1452</v>
       </c>
       <c r="F111" s="59">
@@ -9327,7 +9333,7 @@
       <c r="D112" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="E112" s="92">
+      <c r="E112" s="87">
         <v>1453</v>
       </c>
       <c r="F112" s="44">
@@ -9388,7 +9394,7 @@
         <v>20</v>
       </c>
       <c r="D113" s="38"/>
-      <c r="E113" s="92">
+      <c r="E113" s="87">
         <v>1454</v>
       </c>
       <c r="F113" s="44">
@@ -9447,7 +9453,7 @@
         <v>21</v>
       </c>
       <c r="D114" s="38"/>
-      <c r="E114" s="92">
+      <c r="E114" s="87">
         <v>1455</v>
       </c>
       <c r="F114" s="44">
@@ -9510,7 +9516,7 @@
         <v>22</v>
       </c>
       <c r="D115" s="38"/>
-      <c r="E115" s="92">
+      <c r="E115" s="87">
         <v>1456</v>
       </c>
       <c r="F115" s="44">
@@ -9569,7 +9575,7 @@
         <v>23</v>
       </c>
       <c r="D116" s="38"/>
-      <c r="E116" s="92">
+      <c r="E116" s="87">
         <v>1457</v>
       </c>
       <c r="F116" s="44">
@@ -9630,7 +9636,7 @@
       <c r="D117" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="E117" s="93">
+      <c r="E117" s="88">
         <v>1458</v>
       </c>
       <c r="F117" s="46">
@@ -9752,7 +9758,7 @@
       <c r="D118" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="E118" s="92">
+      <c r="E118" s="87">
         <v>1459</v>
       </c>
       <c r="F118" s="44">
@@ -9811,7 +9817,7 @@
         <v>26</v>
       </c>
       <c r="D119" s="38"/>
-      <c r="E119" s="92">
+      <c r="E119" s="87">
         <v>1460</v>
       </c>
       <c r="F119" s="44">
@@ -9868,7 +9874,7 @@
         <v>27</v>
       </c>
       <c r="D120" s="38"/>
-      <c r="E120" s="92">
+      <c r="E120" s="87">
         <v>1461</v>
       </c>
       <c r="F120" s="44">
@@ -9929,7 +9935,7 @@
         <v>28</v>
       </c>
       <c r="D121" s="38"/>
-      <c r="E121" s="92">
+      <c r="E121" s="87">
         <v>1462</v>
       </c>
       <c r="F121" s="44">
@@ -9988,7 +9994,7 @@
         <v>29</v>
       </c>
       <c r="D122" s="38"/>
-      <c r="E122" s="92">
+      <c r="E122" s="87">
         <v>1463</v>
       </c>
       <c r="F122" s="44">
@@ -10053,7 +10059,7 @@
       <c r="D123" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="E123" s="94">
+      <c r="E123" s="89">
         <v>1464</v>
       </c>
       <c r="F123" s="48">
@@ -10173,7 +10179,7 @@
       <c r="D124" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="E124" s="92">
+      <c r="E124" s="87">
         <v>1466</v>
       </c>
       <c r="F124" s="44">
@@ -10230,7 +10236,7 @@
         <v>2</v>
       </c>
       <c r="D125" s="38"/>
-      <c r="E125" s="92">
+      <c r="E125" s="87">
         <v>1467</v>
       </c>
       <c r="F125" s="44">
@@ -10289,7 +10295,7 @@
         <v>3</v>
       </c>
       <c r="D126" s="38"/>
-      <c r="E126" s="92">
+      <c r="E126" s="87">
         <v>1468</v>
       </c>
       <c r="F126" s="44">
@@ -10350,7 +10356,7 @@
       <c r="D127" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="E127" s="92">
+      <c r="E127" s="87">
         <v>1469</v>
       </c>
       <c r="F127" s="44">
@@ -10411,7 +10417,7 @@
       <c r="D128" s="38" t="s">
         <v>45</v>
       </c>
-      <c r="E128" s="92">
+      <c r="E128" s="87">
         <v>1470</v>
       </c>
       <c r="F128" s="44">
@@ -10472,7 +10478,7 @@
       <c r="D129" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="E129" s="93">
+      <c r="E129" s="88">
         <v>1471</v>
       </c>
       <c r="F129" s="46">
@@ -10590,7 +10596,7 @@
       <c r="D130" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="E130" s="92">
+      <c r="E130" s="87">
         <v>1472</v>
       </c>
       <c r="F130" s="44">
@@ -10649,7 +10655,7 @@
         <v>8</v>
       </c>
       <c r="D131" s="38"/>
-      <c r="E131" s="92">
+      <c r="E131" s="87">
         <v>1473</v>
       </c>
       <c r="F131" s="44">
@@ -10706,7 +10712,7 @@
         <v>9</v>
       </c>
       <c r="D132" s="38"/>
-      <c r="E132" s="92">
+      <c r="E132" s="87">
         <v>1474</v>
       </c>
       <c r="F132" s="44">
@@ -10765,7 +10771,7 @@
         <v>10</v>
       </c>
       <c r="D133" s="38"/>
-      <c r="E133" s="92">
+      <c r="E133" s="87">
         <v>1475</v>
       </c>
       <c r="F133" s="44">
@@ -10824,7 +10830,7 @@
         <v>11</v>
       </c>
       <c r="D134" s="38"/>
-      <c r="E134" s="92">
+      <c r="E134" s="87">
         <v>1476</v>
       </c>
       <c r="F134" s="44">
@@ -10885,7 +10891,7 @@
       <c r="D135" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="E135" s="93">
+      <c r="E135" s="88">
         <v>1477</v>
       </c>
       <c r="F135" s="46">
@@ -11005,7 +11011,7 @@
       <c r="D136" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="E136" s="92">
+      <c r="E136" s="87">
         <v>1478</v>
       </c>
       <c r="F136" s="44">
@@ -11064,7 +11070,7 @@
         <v>14</v>
       </c>
       <c r="D137" s="38"/>
-      <c r="E137" s="92">
+      <c r="E137" s="87">
         <v>1479</v>
       </c>
       <c r="F137" s="44">
@@ -11123,7 +11129,7 @@
         <v>15</v>
       </c>
       <c r="D138" s="38"/>
-      <c r="E138" s="92">
+      <c r="E138" s="87">
         <v>1480</v>
       </c>
       <c r="F138" s="44">
@@ -11182,7 +11188,7 @@
         <v>16</v>
       </c>
       <c r="D139" s="38"/>
-      <c r="E139" s="92">
+      <c r="E139" s="87">
         <v>1481</v>
       </c>
       <c r="F139" s="44">
@@ -11241,7 +11247,7 @@
         <v>17</v>
       </c>
       <c r="D140" s="38"/>
-      <c r="E140" s="95">
+      <c r="E140" s="90">
         <v>1482</v>
       </c>
       <c r="F140" s="4">
@@ -11302,7 +11308,7 @@
       <c r="D141" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="E141" s="96">
+      <c r="E141" s="91">
         <v>1483</v>
       </c>
       <c r="F141" s="46">
@@ -11422,7 +11428,7 @@
       <c r="D142" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="E142" s="92">
+      <c r="E142" s="87">
         <v>1484</v>
       </c>
       <c r="F142" s="44">
@@ -11481,7 +11487,7 @@
         <v>20</v>
       </c>
       <c r="D143" s="38"/>
-      <c r="E143" s="92">
+      <c r="E143" s="87">
         <v>1485</v>
       </c>
       <c r="F143" s="44">
@@ -11540,7 +11546,7 @@
         <v>21</v>
       </c>
       <c r="D144" s="38"/>
-      <c r="E144" s="92">
+      <c r="E144" s="87">
         <v>1486</v>
       </c>
       <c r="F144" s="44">
@@ -11599,7 +11605,7 @@
         <v>22</v>
       </c>
       <c r="D145" s="38"/>
-      <c r="E145" s="92">
+      <c r="E145" s="87">
         <v>1487</v>
       </c>
       <c r="F145" s="44">
@@ -11658,7 +11664,7 @@
         <v>23</v>
       </c>
       <c r="D146" s="38"/>
-      <c r="E146" s="92">
+      <c r="E146" s="87">
         <v>1488</v>
       </c>
       <c r="F146" s="44">
@@ -11717,7 +11723,7 @@
       <c r="D147" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="E147" s="93">
+      <c r="E147" s="88">
         <v>1489</v>
       </c>
       <c r="F147" s="46">
@@ -11839,7 +11845,7 @@
       <c r="D148" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="E148" s="92">
+      <c r="E148" s="87">
         <v>1490</v>
       </c>
       <c r="F148" s="44">
@@ -11898,7 +11904,7 @@
         <v>26</v>
       </c>
       <c r="D149" s="38"/>
-      <c r="E149" s="92">
+      <c r="E149" s="87">
         <v>1491</v>
       </c>
       <c r="F149" s="44">
@@ -11957,7 +11963,7 @@
         <v>27</v>
       </c>
       <c r="D150" s="38"/>
-      <c r="E150" s="92">
+      <c r="E150" s="87">
         <v>1492</v>
       </c>
       <c r="F150" s="44">
@@ -12016,7 +12022,7 @@
         <v>28</v>
       </c>
       <c r="D151" s="38"/>
-      <c r="E151" s="92">
+      <c r="E151" s="87">
         <v>1493</v>
       </c>
       <c r="F151" s="44">
@@ -12077,7 +12083,7 @@
         <v>29</v>
       </c>
       <c r="D152" s="38"/>
-      <c r="E152" s="92">
+      <c r="E152" s="87">
         <v>1494</v>
       </c>
       <c r="F152" s="44">
@@ -12136,7 +12142,7 @@
       <c r="D153" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="E153" s="94">
+      <c r="E153" s="89">
         <v>1495</v>
       </c>
       <c r="F153" s="48">
@@ -12254,7 +12260,7 @@
       <c r="D154" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="E154" s="92">
+      <c r="E154" s="87">
         <v>1497</v>
       </c>
       <c r="F154" s="44">
@@ -12313,7 +12319,7 @@
         <v>2</v>
       </c>
       <c r="D155" s="38"/>
-      <c r="E155" s="92">
+      <c r="E155" s="87">
         <v>1498</v>
       </c>
       <c r="F155" s="44">
@@ -12372,7 +12378,7 @@
         <v>3</v>
       </c>
       <c r="D156" s="38"/>
-      <c r="E156" s="92">
+      <c r="E156" s="87">
         <v>1499</v>
       </c>
       <c r="F156" s="44">
@@ -12431,7 +12437,7 @@
         <v>4</v>
       </c>
       <c r="D157" s="38"/>
-      <c r="E157" s="92">
+      <c r="E157" s="87">
         <v>1500</v>
       </c>
       <c r="F157" s="44">
@@ -12490,7 +12496,7 @@
         <v>5</v>
       </c>
       <c r="D158" s="38"/>
-      <c r="E158" s="92">
+      <c r="E158" s="87">
         <v>1501</v>
       </c>
       <c r="F158" s="44">
@@ -12551,7 +12557,7 @@
       <c r="D159" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="E159" s="93">
+      <c r="E159" s="88">
         <v>1502</v>
       </c>
       <c r="F159" s="46">
@@ -12671,7 +12677,7 @@
       <c r="D160" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="E160" s="92">
+      <c r="E160" s="87">
         <v>1503</v>
       </c>
       <c r="F160" s="44">
@@ -12732,7 +12738,7 @@
         <v>8</v>
       </c>
       <c r="D161" s="38"/>
-      <c r="E161" s="92">
+      <c r="E161" s="87">
         <v>1504</v>
       </c>
       <c r="F161" s="44">
@@ -12791,7 +12797,7 @@
         <v>9</v>
       </c>
       <c r="D162" s="38"/>
-      <c r="E162" s="92">
+      <c r="E162" s="87">
         <v>1505</v>
       </c>
       <c r="F162" s="44">
@@ -12852,7 +12858,7 @@
         <v>10</v>
       </c>
       <c r="D163" s="38"/>
-      <c r="E163" s="92">
+      <c r="E163" s="87">
         <v>1506</v>
       </c>
       <c r="F163" s="44">
@@ -12913,7 +12919,7 @@
         <v>11</v>
       </c>
       <c r="D164" s="38"/>
-      <c r="E164" s="92">
+      <c r="E164" s="87">
         <v>1507</v>
       </c>
       <c r="F164" s="44">
@@ -12976,7 +12982,7 @@
       <c r="D165" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="E165" s="93">
+      <c r="E165" s="88">
         <v>1508</v>
       </c>
       <c r="F165" s="46">
@@ -13096,7 +13102,7 @@
       <c r="D166" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="E166" s="92">
+      <c r="E166" s="87">
         <v>1509</v>
       </c>
       <c r="F166" s="44">
@@ -13157,7 +13163,7 @@
         <v>14</v>
       </c>
       <c r="D167" s="38"/>
-      <c r="E167" s="92">
+      <c r="E167" s="87">
         <v>1510</v>
       </c>
       <c r="F167" s="44">
@@ -13216,7 +13222,7 @@
         <v>15</v>
       </c>
       <c r="D168" s="38"/>
-      <c r="E168" s="92">
+      <c r="E168" s="87">
         <v>1511</v>
       </c>
       <c r="F168" s="44">
@@ -13285,7 +13291,7 @@
         <v>16</v>
       </c>
       <c r="D169" s="38"/>
-      <c r="E169" s="92">
+      <c r="E169" s="87">
         <v>1512</v>
       </c>
       <c r="F169" s="44">
@@ -13346,7 +13352,7 @@
         <v>17</v>
       </c>
       <c r="D170" s="38"/>
-      <c r="E170" s="95">
+      <c r="E170" s="90">
         <v>1513</v>
       </c>
       <c r="F170" s="4">
@@ -13409,7 +13415,7 @@
       <c r="D171" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="E171" s="96">
+      <c r="E171" s="91">
         <v>1514</v>
       </c>
       <c r="F171" s="46">
@@ -13533,7 +13539,7 @@
       <c r="D172" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="E172" s="95">
+      <c r="E172" s="90">
         <v>1515</v>
       </c>
       <c r="F172" s="4">
@@ -13598,7 +13604,7 @@
         <v>20</v>
       </c>
       <c r="D173" s="38"/>
-      <c r="E173" s="95">
+      <c r="E173" s="90">
         <v>1516</v>
       </c>
       <c r="F173" s="4">
@@ -13659,7 +13665,7 @@
         <v>21</v>
       </c>
       <c r="D174" s="38"/>
-      <c r="E174" s="92">
+      <c r="E174" s="87">
         <v>1517</v>
       </c>
       <c r="F174" s="44">
@@ -13718,7 +13724,7 @@
         <v>22</v>
       </c>
       <c r="D175" s="38"/>
-      <c r="E175" s="92">
+      <c r="E175" s="87">
         <v>1518</v>
       </c>
       <c r="F175" s="44">
@@ -13777,7 +13783,7 @@
         <v>23</v>
       </c>
       <c r="D176" s="38"/>
-      <c r="E176" s="92">
+      <c r="E176" s="87">
         <v>1519</v>
       </c>
       <c r="F176" s="44">
@@ -13838,7 +13844,7 @@
       <c r="D177" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="E177" s="93">
+      <c r="E177" s="88">
         <v>1520</v>
       </c>
       <c r="F177" s="46">
@@ -13962,7 +13968,7 @@
       <c r="D178" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="E178" s="92">
+      <c r="E178" s="87">
         <v>1521</v>
       </c>
       <c r="F178" s="44">
@@ -14023,7 +14029,7 @@
         <v>26</v>
       </c>
       <c r="D179" s="38"/>
-      <c r="E179" s="92">
+      <c r="E179" s="87">
         <v>1522</v>
       </c>
       <c r="F179" s="44">
@@ -14082,7 +14088,7 @@
         <v>27</v>
       </c>
       <c r="D180" s="38"/>
-      <c r="E180" s="92">
+      <c r="E180" s="87">
         <v>1523</v>
       </c>
       <c r="F180" s="44">
@@ -14143,7 +14149,7 @@
         <v>28</v>
       </c>
       <c r="D181" s="38"/>
-      <c r="E181" s="92">
+      <c r="E181" s="87">
         <v>1524</v>
       </c>
       <c r="F181" s="44">
@@ -14202,7 +14208,7 @@
         <v>29</v>
       </c>
       <c r="D182" s="38"/>
-      <c r="E182" s="92">
+      <c r="E182" s="87">
         <v>1525</v>
       </c>
       <c r="F182" s="44">
@@ -14265,7 +14271,7 @@
       <c r="D183" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="E183" s="94">
+      <c r="E183" s="89">
         <v>1526</v>
       </c>
       <c r="F183" s="48">
@@ -14385,7 +14391,7 @@
       <c r="D184" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="E184" s="92">
+      <c r="E184" s="87">
         <v>1528</v>
       </c>
       <c r="F184" s="44">
@@ -14442,7 +14448,7 @@
         <v>2</v>
       </c>
       <c r="D185" s="38"/>
-      <c r="E185" s="92">
+      <c r="E185" s="87">
         <v>1529</v>
       </c>
       <c r="F185" s="44">
@@ -14501,7 +14507,7 @@
         <v>3</v>
       </c>
       <c r="D186" s="38"/>
-      <c r="E186" s="92">
+      <c r="E186" s="87">
         <v>1530</v>
       </c>
       <c r="F186" s="44">
@@ -14558,7 +14564,7 @@
         <v>4</v>
       </c>
       <c r="D187" s="38"/>
-      <c r="E187" s="92">
+      <c r="E187" s="87">
         <v>1531</v>
       </c>
       <c r="F187" s="44">
@@ -14615,7 +14621,7 @@
         <v>5</v>
       </c>
       <c r="D188" s="38"/>
-      <c r="E188" s="92">
+      <c r="E188" s="87">
         <v>1532</v>
       </c>
       <c r="F188" s="44">
@@ -14676,7 +14682,7 @@
       <c r="D189" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="E189" s="93">
+      <c r="E189" s="88">
         <v>1533</v>
       </c>
       <c r="F189" s="46">
@@ -14796,7 +14802,7 @@
       <c r="D190" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="E190" s="92">
+      <c r="E190" s="87">
         <v>1534</v>
       </c>
       <c r="F190" s="44">
@@ -14855,7 +14861,7 @@
         <v>8</v>
       </c>
       <c r="D191" s="38"/>
-      <c r="E191" s="92">
+      <c r="E191" s="87">
         <v>1535</v>
       </c>
       <c r="F191" s="44">
@@ -14916,7 +14922,7 @@
         <v>9</v>
       </c>
       <c r="D192" s="38"/>
-      <c r="E192" s="92">
+      <c r="E192" s="87">
         <v>1536</v>
       </c>
       <c r="F192" s="44">
@@ -14975,7 +14981,7 @@
         <v>10</v>
       </c>
       <c r="D193" s="38"/>
-      <c r="E193" s="92">
+      <c r="E193" s="87">
         <v>1537</v>
       </c>
       <c r="F193" s="44">
@@ -15036,7 +15042,7 @@
         <v>11</v>
       </c>
       <c r="D194" s="38"/>
-      <c r="E194" s="92">
+      <c r="E194" s="87">
         <v>1538</v>
       </c>
       <c r="F194" s="44">
@@ -15099,7 +15105,7 @@
       <c r="D195" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="E195" s="93">
+      <c r="E195" s="88">
         <v>1539</v>
       </c>
       <c r="F195" s="46">
@@ -15219,7 +15225,7 @@
       <c r="D196" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="E196" s="92">
+      <c r="E196" s="87">
         <v>1540</v>
       </c>
       <c r="F196" s="44">
@@ -15282,7 +15288,7 @@
         <v>14</v>
       </c>
       <c r="D197" s="38"/>
-      <c r="E197" s="92">
+      <c r="E197" s="87">
         <v>1541</v>
       </c>
       <c r="F197" s="44">
@@ -15345,7 +15351,7 @@
         <v>15</v>
       </c>
       <c r="D198" s="38"/>
-      <c r="E198" s="95">
+      <c r="E198" s="90">
         <v>1542</v>
       </c>
       <c r="F198" s="4">
@@ -15404,7 +15410,7 @@
         <v>16</v>
       </c>
       <c r="D199" s="38"/>
-      <c r="E199" s="95">
+      <c r="E199" s="90">
         <v>1543</v>
       </c>
       <c r="F199" s="4">
@@ -15467,7 +15473,7 @@
         <v>17</v>
       </c>
       <c r="D200" s="38"/>
-      <c r="E200" s="95">
+      <c r="E200" s="90">
         <v>1544</v>
       </c>
       <c r="F200" s="4">
@@ -15532,7 +15538,7 @@
       <c r="D201" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="E201" s="96">
+      <c r="E201" s="91">
         <v>1545</v>
       </c>
       <c r="F201" s="46">
@@ -15650,7 +15656,7 @@
       <c r="D202" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="E202" s="95">
+      <c r="E202" s="90">
         <v>1546</v>
       </c>
       <c r="F202" s="4">
@@ -15717,7 +15723,7 @@
       <c r="D203" s="38" t="s">
         <v>45</v>
       </c>
-      <c r="E203" s="95">
+      <c r="E203" s="90">
         <v>1547</v>
       </c>
       <c r="F203" s="4">
@@ -15780,7 +15786,7 @@
       <c r="D204" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="E204" s="95">
+      <c r="E204" s="90">
         <v>1548</v>
       </c>
       <c r="F204" s="4">
@@ -15843,7 +15849,7 @@
       <c r="D205" s="38" t="s">
         <v>46</v>
       </c>
-      <c r="E205" s="95">
+      <c r="E205" s="90">
         <v>1549</v>
       </c>
       <c r="F205" s="4">
@@ -15902,7 +15908,7 @@
       <c r="D206" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="E206" s="95">
+      <c r="E206" s="90">
         <v>1550</v>
       </c>
       <c r="F206" s="4">
@@ -15961,7 +15967,7 @@
       <c r="D207" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="E207" s="96">
+      <c r="E207" s="91">
         <v>1551</v>
       </c>
       <c r="F207" s="21">
@@ -16085,7 +16091,7 @@
       <c r="D208" s="38" t="s">
         <v>46</v>
       </c>
-      <c r="E208" s="92">
+      <c r="E208" s="87">
         <v>1552</v>
       </c>
       <c r="F208" s="44">
@@ -16144,7 +16150,7 @@
       <c r="D209" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="E209" s="92">
+      <c r="E209" s="87">
         <v>1553</v>
       </c>
       <c r="F209" s="44">
@@ -16203,7 +16209,7 @@
       <c r="D210" s="38" t="s">
         <v>46</v>
       </c>
-      <c r="E210" s="92">
+      <c r="E210" s="87">
         <v>1554</v>
       </c>
       <c r="F210" s="44">
@@ -16264,7 +16270,7 @@
       <c r="D211" s="38" t="s">
         <v>45</v>
       </c>
-      <c r="E211" s="92">
+      <c r="E211" s="87">
         <v>1555</v>
       </c>
       <c r="F211" s="44">
@@ -16323,7 +16329,7 @@
       <c r="D212" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="E212" s="92">
+      <c r="E212" s="87">
         <v>1556</v>
       </c>
       <c r="F212" s="44">
@@ -16392,7 +16398,7 @@
       <c r="D213" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="E213" s="94">
+      <c r="E213" s="89">
         <v>1557</v>
       </c>
       <c r="F213" s="48">
@@ -16510,7 +16516,7 @@
       <c r="D214" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="E214" s="92">
+      <c r="E214" s="87">
         <v>1560</v>
       </c>
       <c r="F214" s="44">
@@ -16571,7 +16577,7 @@
         <v>2</v>
       </c>
       <c r="D215" s="38"/>
-      <c r="E215" s="92">
+      <c r="E215" s="87">
         <v>1561</v>
       </c>
       <c r="F215" s="44">
@@ -16634,7 +16640,7 @@
       <c r="D216" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="E216" s="92">
+      <c r="E216" s="87">
         <v>1562</v>
       </c>
       <c r="F216" s="44">
@@ -16695,7 +16701,7 @@
       <c r="D217" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="E217" s="92">
+      <c r="E217" s="87">
         <v>1563</v>
       </c>
       <c r="F217" s="44">
@@ -16758,7 +16764,7 @@
         <v>5</v>
       </c>
       <c r="D218" s="38"/>
-      <c r="E218" s="92">
+      <c r="E218" s="87">
         <v>1564</v>
       </c>
       <c r="F218" s="44">
@@ -16821,7 +16827,7 @@
       <c r="D219" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="E219" s="93">
+      <c r="E219" s="88">
         <v>1565</v>
       </c>
       <c r="F219" s="46">
@@ -16941,7 +16947,7 @@
       <c r="D220" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="E220" s="92">
+      <c r="E220" s="87">
         <v>1566</v>
       </c>
       <c r="F220" s="44">
@@ -17000,7 +17006,7 @@
         <v>8</v>
       </c>
       <c r="D221" s="38"/>
-      <c r="E221" s="92">
+      <c r="E221" s="87">
         <v>1567</v>
       </c>
       <c r="F221" s="44">
@@ -17061,7 +17067,7 @@
       <c r="D222" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="E222" s="92">
+      <c r="E222" s="87">
         <v>1568</v>
       </c>
       <c r="F222" s="44">
@@ -17120,7 +17126,7 @@
       <c r="D223" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="E223" s="92">
+      <c r="E223" s="87">
         <v>1571</v>
       </c>
       <c r="F223" s="44">
@@ -17183,7 +17189,7 @@
         <v>11</v>
       </c>
       <c r="D224" s="38"/>
-      <c r="E224" s="92">
+      <c r="E224" s="87">
         <v>1572</v>
       </c>
       <c r="F224" s="44">
@@ -17248,7 +17254,7 @@
       <c r="D225" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="E225" s="93">
+      <c r="E225" s="88">
         <v>1573</v>
       </c>
       <c r="F225" s="46">
@@ -17366,7 +17372,7 @@
       <c r="D226" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="E226" s="92">
+      <c r="E226" s="87">
         <v>1574</v>
       </c>
       <c r="F226" s="44">
@@ -17431,7 +17437,7 @@
         <v>14</v>
       </c>
       <c r="D227" s="38"/>
-      <c r="E227" s="92">
+      <c r="E227" s="87">
         <v>1575</v>
       </c>
       <c r="F227" s="44">
@@ -17490,7 +17496,7 @@
         <v>15</v>
       </c>
       <c r="D228" s="38"/>
-      <c r="E228" s="92">
+      <c r="E228" s="87">
         <v>1576</v>
       </c>
       <c r="F228" s="44">
@@ -17547,7 +17553,7 @@
         <v>16</v>
       </c>
       <c r="D229" s="38"/>
-      <c r="E229" s="92">
+      <c r="E229" s="87">
         <v>1577</v>
       </c>
       <c r="F229" s="44">
@@ -17606,7 +17612,7 @@
         <v>17</v>
       </c>
       <c r="D230" s="38"/>
-      <c r="E230" s="92">
+      <c r="E230" s="87">
         <v>1578</v>
       </c>
       <c r="F230" s="44">
@@ -17667,7 +17673,7 @@
       <c r="D231" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="E231" s="96">
+      <c r="E231" s="91">
         <v>1579</v>
       </c>
       <c r="F231" s="46">
@@ -17785,7 +17791,7 @@
       <c r="D232" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="E232" s="95">
+      <c r="E232" s="90">
         <v>1580</v>
       </c>
       <c r="F232" s="4">
@@ -17844,7 +17850,7 @@
         <v>20</v>
       </c>
       <c r="D233" s="38"/>
-      <c r="E233" s="92">
+      <c r="E233" s="87">
         <v>1581</v>
       </c>
       <c r="F233" s="44">
@@ -17907,7 +17913,7 @@
         <v>21</v>
       </c>
       <c r="D234" s="38"/>
-      <c r="E234" s="92">
+      <c r="E234" s="87">
         <v>1582</v>
       </c>
       <c r="F234" s="44">
@@ -17970,7 +17976,7 @@
         <v>22</v>
       </c>
       <c r="D235" s="38"/>
-      <c r="E235" s="92">
+      <c r="E235" s="87">
         <v>1583</v>
       </c>
       <c r="F235" s="44">
@@ -18029,7 +18035,7 @@
         <v>23</v>
       </c>
       <c r="D236" s="38"/>
-      <c r="E236" s="92">
+      <c r="E236" s="87">
         <v>1584</v>
       </c>
       <c r="F236" s="44">
@@ -18090,7 +18096,7 @@
       <c r="D237" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="E237" s="93">
+      <c r="E237" s="88">
         <v>1585</v>
       </c>
       <c r="F237" s="46">
@@ -18208,7 +18214,7 @@
       <c r="D238" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="E238" s="92">
+      <c r="E238" s="87">
         <v>1586</v>
       </c>
       <c r="F238" s="44">
@@ -18267,7 +18273,7 @@
         <v>26</v>
       </c>
       <c r="D239" s="38"/>
-      <c r="E239" s="92">
+      <c r="E239" s="87">
         <v>1587</v>
       </c>
       <c r="F239" s="44">
@@ -18326,7 +18332,7 @@
         <v>27</v>
       </c>
       <c r="D240" s="38"/>
-      <c r="E240" s="92">
+      <c r="E240" s="87">
         <v>1588</v>
       </c>
       <c r="F240" s="44">
@@ -18385,7 +18391,7 @@
         <v>28</v>
       </c>
       <c r="D241" s="38"/>
-      <c r="E241" s="92">
+      <c r="E241" s="87">
         <v>1589</v>
       </c>
       <c r="F241" s="44">
@@ -18444,7 +18450,7 @@
         <v>29</v>
       </c>
       <c r="D242" s="38"/>
-      <c r="E242" s="92">
+      <c r="E242" s="87">
         <v>1590</v>
       </c>
       <c r="F242" s="44">
@@ -18505,7 +18511,7 @@
       <c r="D243" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="E243" s="94">
+      <c r="E243" s="89">
         <v>1591</v>
       </c>
       <c r="F243" s="48">
@@ -19784,7 +19790,7 @@
       <c r="D261" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="E261" s="97">
+      <c r="E261" s="92">
         <v>1610</v>
       </c>
       <c r="F261" s="46">
@@ -19900,7 +19906,7 @@
       <c r="D262" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="E262" s="98">
+      <c r="E262" s="93">
         <v>1611</v>
       </c>
       <c r="F262" s="4">
@@ -21899,7 +21905,7 @@
       <c r="D291" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="E291" s="97">
+      <c r="E291" s="92">
         <v>1642</v>
       </c>
       <c r="F291" s="46">
@@ -22019,7 +22025,7 @@
       <c r="D292" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="E292" s="98">
+      <c r="E292" s="93">
         <v>1643</v>
       </c>
       <c r="F292" s="4">
@@ -24010,7 +24016,7 @@
       <c r="D321" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="E321" s="97">
+      <c r="E321" s="92">
         <v>1673</v>
       </c>
       <c r="F321" s="46">
@@ -24134,7 +24140,7 @@
       <c r="D322" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="E322" s="98">
+      <c r="E322" s="93">
         <v>1674</v>
       </c>
       <c r="F322" s="4">
@@ -26139,7 +26145,7 @@
       <c r="D351" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="E351" s="97">
+      <c r="E351" s="92">
         <v>1694</v>
       </c>
       <c r="F351" s="46">
@@ -26257,7 +26263,7 @@
       <c r="D352" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="E352" s="98">
+      <c r="E352" s="93">
         <v>1695</v>
       </c>
       <c r="F352" s="4">
@@ -28236,7 +28242,7 @@
       <c r="D381" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="E381" s="97">
+      <c r="E381" s="92">
         <v>1748</v>
       </c>
       <c r="F381" s="46">
@@ -28354,7 +28360,7 @@
       <c r="D382" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="E382" s="98">
+      <c r="E382" s="93">
         <v>1749</v>
       </c>
       <c r="F382" s="4">
@@ -30361,7 +30367,7 @@
       <c r="D411" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="E411" s="97">
+      <c r="E411" s="92">
         <v>1780</v>
       </c>
       <c r="F411" s="46">
@@ -30481,7 +30487,7 @@
       <c r="D412" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="E412" s="98">
+      <c r="E412" s="93">
         <v>1781</v>
       </c>
       <c r="F412" s="4">
@@ -35485,7 +35491,7 @@
       <c r="D483" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="E483" s="97">
+      <c r="E483" s="92">
         <v>1854</v>
       </c>
       <c r="F483" s="48">
@@ -37610,7 +37616,7 @@
       <c r="D513" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="E513" s="97">
+      <c r="E513" s="92">
         <v>1885</v>
       </c>
       <c r="F513" s="48">
@@ -39703,7 +39709,7 @@
       <c r="D543" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="E543" s="99">
+      <c r="E543" s="94">
         <v>1916</v>
       </c>
       <c r="F543" s="48">
@@ -41584,7 +41590,7 @@
       <c r="D573" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="E573" s="99">
+      <c r="E573" s="94">
         <v>1947</v>
       </c>
       <c r="F573" s="48">
@@ -55056,7 +55062,7 @@
       <c r="D771" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="E771" s="97" t="s">
+      <c r="E771" s="92" t="s">
         <v>129</v>
       </c>
       <c r="F771" s="81">
@@ -55117,7 +55123,7 @@
       <c r="D772" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="E772" s="98" t="s">
+      <c r="E772" s="93" t="s">
         <v>129</v>
       </c>
       <c r="F772" s="81">
@@ -63225,442 +63231,442 @@
       </c>
     </row>
     <row r="904" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="E904" s="100"/>
+      <c r="E904" s="95"/>
     </row>
     <row r="905" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="E905" s="100"/>
+      <c r="E905" s="95"/>
     </row>
     <row r="906" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="E906" s="100"/>
+      <c r="E906" s="95"/>
     </row>
     <row r="907" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="E907" s="100"/>
+      <c r="E907" s="95"/>
     </row>
     <row r="908" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="E908" s="100"/>
+      <c r="E908" s="95"/>
     </row>
     <row r="909" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="E909" s="100"/>
+      <c r="E909" s="95"/>
     </row>
     <row r="910" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="E910" s="100"/>
+      <c r="E910" s="95"/>
     </row>
     <row r="911" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="E911" s="100"/>
+      <c r="E911" s="95"/>
     </row>
     <row r="912" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="E912" s="100"/>
+      <c r="E912" s="95"/>
     </row>
     <row r="913" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E913" s="100"/>
+      <c r="E913" s="95"/>
     </row>
     <row r="914" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E914" s="100"/>
+      <c r="E914" s="95"/>
     </row>
     <row r="915" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E915" s="100"/>
+      <c r="E915" s="95"/>
     </row>
     <row r="916" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E916" s="100"/>
+      <c r="E916" s="95"/>
     </row>
     <row r="917" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E917" s="100"/>
+      <c r="E917" s="95"/>
     </row>
     <row r="918" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E918" s="100"/>
+      <c r="E918" s="95"/>
     </row>
     <row r="919" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E919" s="100"/>
+      <c r="E919" s="95"/>
     </row>
     <row r="920" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E920" s="100"/>
+      <c r="E920" s="95"/>
     </row>
     <row r="921" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E921" s="100"/>
+      <c r="E921" s="95"/>
     </row>
     <row r="922" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E922" s="100"/>
+      <c r="E922" s="95"/>
     </row>
     <row r="923" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E923" s="100"/>
+      <c r="E923" s="95"/>
     </row>
     <row r="924" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E924" s="100"/>
+      <c r="E924" s="95"/>
     </row>
     <row r="925" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E925" s="100"/>
+      <c r="E925" s="95"/>
     </row>
     <row r="926" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E926" s="100"/>
+      <c r="E926" s="95"/>
     </row>
     <row r="927" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E927" s="100"/>
+      <c r="E927" s="95"/>
     </row>
     <row r="928" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E928" s="100"/>
+      <c r="E928" s="95"/>
     </row>
     <row r="929" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E929" s="100"/>
+      <c r="E929" s="95"/>
     </row>
     <row r="930" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E930" s="100"/>
+      <c r="E930" s="95"/>
     </row>
     <row r="931" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E931" s="100"/>
+      <c r="E931" s="95"/>
     </row>
     <row r="932" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E932" s="100"/>
+      <c r="E932" s="95"/>
     </row>
     <row r="933" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E933" s="100"/>
+      <c r="E933" s="95"/>
     </row>
     <row r="934" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E934" s="100"/>
+      <c r="E934" s="95"/>
     </row>
     <row r="935" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E935" s="100"/>
+      <c r="E935" s="95"/>
     </row>
     <row r="936" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E936" s="100"/>
+      <c r="E936" s="95"/>
     </row>
     <row r="937" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E937" s="100"/>
+      <c r="E937" s="95"/>
     </row>
     <row r="938" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E938" s="100"/>
+      <c r="E938" s="95"/>
     </row>
     <row r="939" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E939" s="100"/>
+      <c r="E939" s="95"/>
     </row>
     <row r="940" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E940" s="100"/>
+      <c r="E940" s="95"/>
     </row>
     <row r="941" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E941" s="100"/>
+      <c r="E941" s="95"/>
     </row>
     <row r="942" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E942" s="100"/>
+      <c r="E942" s="95"/>
     </row>
     <row r="943" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E943" s="100"/>
+      <c r="E943" s="95"/>
     </row>
     <row r="944" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E944" s="100"/>
+      <c r="E944" s="95"/>
     </row>
     <row r="945" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E945" s="100"/>
+      <c r="E945" s="95"/>
     </row>
     <row r="946" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E946" s="100"/>
+      <c r="E946" s="95"/>
     </row>
     <row r="947" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E947" s="100"/>
+      <c r="E947" s="95"/>
     </row>
     <row r="948" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E948" s="100"/>
+      <c r="E948" s="95"/>
     </row>
     <row r="949" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E949" s="100"/>
+      <c r="E949" s="95"/>
     </row>
     <row r="950" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E950" s="100"/>
+      <c r="E950" s="95"/>
     </row>
     <row r="951" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E951" s="100"/>
+      <c r="E951" s="95"/>
     </row>
     <row r="952" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E952" s="100"/>
+      <c r="E952" s="95"/>
     </row>
     <row r="953" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E953" s="100"/>
+      <c r="E953" s="95"/>
     </row>
     <row r="954" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E954" s="100"/>
+      <c r="E954" s="95"/>
     </row>
     <row r="955" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E955" s="100"/>
+      <c r="E955" s="95"/>
     </row>
     <row r="956" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E956" s="100"/>
+      <c r="E956" s="95"/>
     </row>
     <row r="957" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E957" s="100"/>
+      <c r="E957" s="95"/>
     </row>
     <row r="958" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E958" s="100"/>
+      <c r="E958" s="95"/>
     </row>
     <row r="959" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E959" s="100"/>
+      <c r="E959" s="95"/>
     </row>
     <row r="960" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E960" s="100"/>
+      <c r="E960" s="95"/>
     </row>
     <row r="961" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E961" s="100"/>
+      <c r="E961" s="95"/>
     </row>
     <row r="962" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E962" s="100"/>
+      <c r="E962" s="95"/>
     </row>
     <row r="963" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E963" s="100"/>
+      <c r="E963" s="95"/>
     </row>
     <row r="964" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E964" s="100"/>
+      <c r="E964" s="95"/>
     </row>
     <row r="965" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E965" s="100"/>
+      <c r="E965" s="95"/>
     </row>
     <row r="966" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E966" s="100"/>
+      <c r="E966" s="95"/>
     </row>
     <row r="967" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E967" s="100"/>
+      <c r="E967" s="95"/>
     </row>
     <row r="968" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E968" s="100"/>
+      <c r="E968" s="95"/>
     </row>
     <row r="969" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E969" s="100"/>
+      <c r="E969" s="95"/>
     </row>
     <row r="970" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E970" s="100"/>
+      <c r="E970" s="95"/>
     </row>
     <row r="971" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E971" s="100"/>
+      <c r="E971" s="95"/>
     </row>
     <row r="972" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E972" s="100"/>
+      <c r="E972" s="95"/>
     </row>
     <row r="973" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E973" s="100"/>
+      <c r="E973" s="95"/>
     </row>
     <row r="974" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E974" s="100"/>
+      <c r="E974" s="95"/>
     </row>
     <row r="975" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E975" s="100"/>
+      <c r="E975" s="95"/>
     </row>
     <row r="976" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E976" s="100"/>
+      <c r="E976" s="95"/>
     </row>
     <row r="977" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E977" s="100"/>
+      <c r="E977" s="95"/>
     </row>
     <row r="978" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E978" s="100"/>
+      <c r="E978" s="95"/>
     </row>
     <row r="979" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E979" s="100"/>
+      <c r="E979" s="95"/>
     </row>
     <row r="980" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E980" s="100"/>
+      <c r="E980" s="95"/>
     </row>
     <row r="981" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E981" s="100"/>
+      <c r="E981" s="95"/>
     </row>
     <row r="982" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E982" s="100"/>
+      <c r="E982" s="95"/>
     </row>
     <row r="983" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E983" s="100"/>
+      <c r="E983" s="95"/>
     </row>
     <row r="984" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E984" s="100"/>
+      <c r="E984" s="95"/>
     </row>
     <row r="985" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E985" s="100"/>
+      <c r="E985" s="95"/>
     </row>
     <row r="986" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E986" s="100"/>
+      <c r="E986" s="95"/>
     </row>
     <row r="987" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E987" s="100"/>
+      <c r="E987" s="95"/>
     </row>
     <row r="988" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E988" s="100"/>
+      <c r="E988" s="95"/>
     </row>
     <row r="989" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E989" s="100"/>
+      <c r="E989" s="95"/>
     </row>
     <row r="990" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E990" s="100"/>
+      <c r="E990" s="95"/>
     </row>
     <row r="991" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E991" s="100"/>
+      <c r="E991" s="95"/>
     </row>
     <row r="992" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E992" s="100"/>
+      <c r="E992" s="95"/>
     </row>
     <row r="993" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E993" s="100"/>
+      <c r="E993" s="95"/>
     </row>
     <row r="994" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E994" s="100"/>
+      <c r="E994" s="95"/>
     </row>
     <row r="995" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E995" s="100"/>
+      <c r="E995" s="95"/>
     </row>
     <row r="996" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E996" s="100"/>
+      <c r="E996" s="95"/>
     </row>
     <row r="997" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E997" s="100"/>
+      <c r="E997" s="95"/>
     </row>
     <row r="998" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E998" s="100"/>
+      <c r="E998" s="95"/>
     </row>
     <row r="999" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E999" s="100"/>
+      <c r="E999" s="95"/>
     </row>
     <row r="1000" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E1000" s="100"/>
+      <c r="E1000" s="95"/>
     </row>
     <row r="1001" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E1001" s="100"/>
+      <c r="E1001" s="95"/>
     </row>
     <row r="1002" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E1002" s="100"/>
+      <c r="E1002" s="95"/>
     </row>
     <row r="1003" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E1003" s="100"/>
+      <c r="E1003" s="95"/>
     </row>
     <row r="1004" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E1004" s="100"/>
+      <c r="E1004" s="95"/>
     </row>
     <row r="1005" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E1005" s="100"/>
+      <c r="E1005" s="95"/>
     </row>
     <row r="1006" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E1006" s="100"/>
+      <c r="E1006" s="95"/>
     </row>
     <row r="1007" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E1007" s="100"/>
+      <c r="E1007" s="95"/>
     </row>
     <row r="1008" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E1008" s="100"/>
+      <c r="E1008" s="95"/>
     </row>
     <row r="1009" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E1009" s="100"/>
+      <c r="E1009" s="95"/>
     </row>
     <row r="1010" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E1010" s="100"/>
+      <c r="E1010" s="95"/>
     </row>
     <row r="1011" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E1011" s="100"/>
+      <c r="E1011" s="95"/>
     </row>
     <row r="1012" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E1012" s="100"/>
+      <c r="E1012" s="95"/>
     </row>
     <row r="1013" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E1013" s="100"/>
+      <c r="E1013" s="95"/>
     </row>
     <row r="1014" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E1014" s="100"/>
+      <c r="E1014" s="95"/>
     </row>
     <row r="1015" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E1015" s="100"/>
+      <c r="E1015" s="95"/>
     </row>
     <row r="1016" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E1016" s="100"/>
+      <c r="E1016" s="95"/>
     </row>
     <row r="1017" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E1017" s="100"/>
+      <c r="E1017" s="95"/>
     </row>
     <row r="1018" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E1018" s="100"/>
+      <c r="E1018" s="95"/>
     </row>
     <row r="1019" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E1019" s="100"/>
+      <c r="E1019" s="95"/>
     </row>
     <row r="1020" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E1020" s="100"/>
+      <c r="E1020" s="95"/>
     </row>
     <row r="1021" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E1021" s="100"/>
+      <c r="E1021" s="95"/>
     </row>
     <row r="1022" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E1022" s="100"/>
+      <c r="E1022" s="95"/>
     </row>
     <row r="1023" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E1023" s="100"/>
+      <c r="E1023" s="95"/>
     </row>
     <row r="1024" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E1024" s="100"/>
+      <c r="E1024" s="95"/>
     </row>
     <row r="1025" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E1025" s="100"/>
+      <c r="E1025" s="95"/>
     </row>
     <row r="1026" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E1026" s="100"/>
+      <c r="E1026" s="95"/>
     </row>
     <row r="1027" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E1027" s="100"/>
+      <c r="E1027" s="95"/>
     </row>
     <row r="1028" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E1028" s="100"/>
+      <c r="E1028" s="95"/>
     </row>
     <row r="1029" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E1029" s="100"/>
+      <c r="E1029" s="95"/>
     </row>
     <row r="1030" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E1030" s="100"/>
+      <c r="E1030" s="95"/>
     </row>
     <row r="1031" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E1031" s="100"/>
+      <c r="E1031" s="95"/>
     </row>
     <row r="1032" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E1032" s="100"/>
+      <c r="E1032" s="95"/>
     </row>
     <row r="1033" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E1033" s="100"/>
+      <c r="E1033" s="95"/>
     </row>
     <row r="1034" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E1034" s="100"/>
+      <c r="E1034" s="95"/>
     </row>
     <row r="1035" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E1035" s="100"/>
+      <c r="E1035" s="95"/>
     </row>
     <row r="1036" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E1036" s="100"/>
+      <c r="E1036" s="95"/>
     </row>
     <row r="1037" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E1037" s="100"/>
+      <c r="E1037" s="95"/>
     </row>
     <row r="1038" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E1038" s="100"/>
+      <c r="E1038" s="95"/>
     </row>
     <row r="1039" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E1039" s="100"/>
+      <c r="E1039" s="95"/>
     </row>
     <row r="1040" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E1040" s="100"/>
+      <c r="E1040" s="95"/>
     </row>
     <row r="1041" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E1041" s="100"/>
+      <c r="E1041" s="95"/>
     </row>
     <row r="1042" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E1042" s="100"/>
+      <c r="E1042" s="95"/>
     </row>
     <row r="1043" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E1043" s="100"/>
+      <c r="E1043" s="95"/>
     </row>
     <row r="1044" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E1044" s="100"/>
+      <c r="E1044" s="95"/>
     </row>
     <row r="1045" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E1045" s="100"/>
+      <c r="E1045" s="95"/>
     </row>
     <row r="1046" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E1046" s="100"/>
+      <c r="E1046" s="95"/>
     </row>
     <row r="1047" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E1047" s="100"/>
+      <c r="E1047" s="95"/>
     </row>
     <row r="1048" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E1048" s="100"/>
+      <c r="E1048" s="95"/>
     </row>
     <row r="1049" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E1049" s="100"/>
+      <c r="E1049" s="95"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -63676,1021 +63682,1145 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:L37"/>
+  <dimension ref="A1:M37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="7.33203125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="8.6640625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" style="3"/>
-    <col min="4" max="4" width="13.1640625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="19.5" style="3" customWidth="1"/>
-    <col min="6" max="6" width="18.5" style="3" customWidth="1"/>
-    <col min="7" max="7" width="18.1640625" style="3" customWidth="1"/>
-    <col min="8" max="8" width="14.5" style="3" customWidth="1"/>
-    <col min="9" max="9" width="37.33203125" customWidth="1"/>
-    <col min="11" max="11" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.33203125" style="86" customWidth="1"/>
+    <col min="3" max="3" width="8.6640625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" style="3"/>
+    <col min="5" max="5" width="13.1640625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="19.5" style="3" customWidth="1"/>
+    <col min="7" max="7" width="18.5" style="3" customWidth="1"/>
+    <col min="8" max="8" width="18.1640625" style="3" customWidth="1"/>
+    <col min="9" max="9" width="14.5" style="3" customWidth="1"/>
+    <col min="10" max="10" width="37.33203125" customWidth="1"/>
+    <col min="12" max="12" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="63" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="64" t="s">
+        <v>146</v>
+      </c>
+      <c r="C1" s="64" t="s">
         <v>58</v>
       </c>
-      <c r="C1" s="64" t="s">
+      <c r="D1" s="64" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="64" t="s">
+      <c r="E1" s="64" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="64" t="s">
+      <c r="F1" s="64" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="64" t="s">
+      <c r="G1" s="64" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="64" t="s">
+      <c r="H1" s="64" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="64" t="s">
+      <c r="I1" s="64" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="65" t="s">
+      <c r="J1" s="65" t="s">
         <v>15</v>
       </c>
-      <c r="K1" s="91" t="s">
+      <c r="L1" s="101" t="s">
         <v>26</v>
       </c>
-      <c r="L1" s="91"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M1" s="101"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="70">
         <v>1</v>
       </c>
       <c r="B2" s="71">
+        <f>VLOOKUP(A2,'Order Chrono-Riviere'!$A$2:$B$31,2,FALSE)</f>
+        <v>9</v>
+      </c>
+      <c r="C2" s="71">
         <v>1433</v>
       </c>
-      <c r="C2" s="72">
+      <c r="D2" s="72">
         <v>42979</v>
       </c>
-      <c r="D2" s="73">
+      <c r="E2" s="73">
         <v>0.66388888888888886</v>
       </c>
-      <c r="E2" s="74">
-        <v>1</v>
-      </c>
       <c r="F2" s="74">
         <v>1</v>
       </c>
-      <c r="G2" s="71">
+      <c r="G2" s="74">
+        <v>1</v>
+      </c>
+      <c r="H2" s="71">
         <v>1766</v>
       </c>
-      <c r="H2" s="75">
-        <f>G2/30</f>
+      <c r="I2" s="75">
+        <f>H2/30</f>
         <v>58.866666666666667</v>
       </c>
-      <c r="I2" s="76" t="s">
+      <c r="J2" s="76" t="s">
         <v>36</v>
       </c>
-      <c r="K2" s="14">
-        <f>AVERAGE(G2:G28)</f>
+      <c r="L2" s="14">
+        <f>AVERAGE(H2:H28)</f>
         <v>1625.7692307692307</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="11">
         <v>2</v>
       </c>
-      <c r="B3" s="69">
+      <c r="B3" s="4">
+        <f>VLOOKUP(A3,'Order Chrono-Riviere'!$A$2:$B$31,2,FALSE)</f>
+        <v>12</v>
+      </c>
+      <c r="C3" s="69">
         <v>1363</v>
       </c>
-      <c r="C3" s="66">
+      <c r="D3" s="66">
         <v>42980</v>
       </c>
-      <c r="D3" s="67">
+      <c r="E3" s="67">
         <v>0.41666666666666669</v>
       </c>
-      <c r="E3" s="68">
+      <c r="F3" s="68">
         <v>0.1</v>
       </c>
-      <c r="F3" s="68">
+      <c r="G3" s="68">
         <v>0</v>
       </c>
-      <c r="G3" s="4">
+      <c r="H3" s="4">
         <v>1550</v>
       </c>
-      <c r="H3" s="69">
-        <f>G3/30</f>
+      <c r="I3" s="69">
+        <f>H3/30</f>
         <v>51.666666666666664</v>
       </c>
-      <c r="I3" s="77" t="s">
+      <c r="J3" s="77" t="s">
         <v>113</v>
       </c>
-      <c r="K3" s="91" t="s">
+      <c r="L3" s="101" t="s">
         <v>27</v>
       </c>
-      <c r="L3" s="91"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M3" s="101"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="11">
         <v>3</v>
       </c>
       <c r="B4" s="4">
+        <f>VLOOKUP(A4,'Order Chrono-Riviere'!$A$2:$B$31,2,FALSE)</f>
+        <v>13</v>
+      </c>
+      <c r="C4" s="4">
         <v>1402</v>
       </c>
-      <c r="C4" s="66">
+      <c r="D4" s="66">
         <v>42980</v>
       </c>
-      <c r="D4" s="67">
+      <c r="E4" s="67">
         <v>0.58472222222222225</v>
-      </c>
-      <c r="E4" s="68">
-        <v>0</v>
       </c>
       <c r="F4" s="68">
         <v>0</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4" s="68">
+        <v>0</v>
+      </c>
+      <c r="H4" s="4">
         <v>1794</v>
       </c>
-      <c r="H4" s="69">
-        <f>G4/30</f>
+      <c r="I4" s="69">
+        <f>H4/30</f>
         <v>59.8</v>
       </c>
-      <c r="I4" s="77" t="s">
+      <c r="J4" s="77" t="s">
         <v>42</v>
       </c>
-      <c r="K4" s="14">
-        <f>STDEV(G2:G30)</f>
+      <c r="L4" s="14">
+        <f>STDEV(H2:H30)</f>
         <v>83.990047281377585</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="11">
         <v>4</v>
       </c>
       <c r="B5" s="4">
+        <f>VLOOKUP(A5,'Order Chrono-Riviere'!$A$2:$B$31,2,FALSE)</f>
+        <v>18</v>
+      </c>
+      <c r="C5" s="4">
         <v>1434</v>
       </c>
-      <c r="C5" s="66">
+      <c r="D5" s="66">
         <v>42981</v>
       </c>
-      <c r="D5" s="67">
+      <c r="E5" s="67">
         <v>0.40277777777777773</v>
-      </c>
-      <c r="E5" s="68">
-        <v>0</v>
       </c>
       <c r="F5" s="68">
         <v>0</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5" s="68">
+        <v>0</v>
+      </c>
+      <c r="H5" s="4">
         <v>1651</v>
       </c>
-      <c r="H5" s="69">
-        <f t="shared" ref="H5:H11" si="0">G5/30</f>
+      <c r="I5" s="69">
+        <f t="shared" ref="I5:I11" si="0">H5/30</f>
         <v>55.033333333333331</v>
       </c>
-      <c r="I5" s="77" t="s">
+      <c r="J5" s="77" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="11">
         <v>5</v>
       </c>
       <c r="B6" s="4">
+        <f>VLOOKUP(A6,'Order Chrono-Riviere'!$A$2:$B$31,2,FALSE)</f>
+        <v>19</v>
+      </c>
+      <c r="C6" s="4">
         <v>1465</v>
       </c>
-      <c r="C6" s="66">
+      <c r="D6" s="66">
         <v>42981</v>
       </c>
-      <c r="D6" s="67">
+      <c r="E6" s="67">
         <v>0.52361111111111114</v>
-      </c>
-      <c r="E6" s="68">
-        <v>0</v>
       </c>
       <c r="F6" s="68">
         <v>0</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6" s="68">
+        <v>0</v>
+      </c>
+      <c r="H6" s="4">
         <v>1601</v>
       </c>
-      <c r="H6" s="69">
+      <c r="I6" s="69">
         <f t="shared" si="0"/>
         <v>53.366666666666667</v>
       </c>
-      <c r="I6" s="77" t="s">
+      <c r="J6" s="77" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="11">
         <v>6</v>
       </c>
       <c r="B7" s="4">
+        <f>VLOOKUP(A7,'Order Chrono-Riviere'!$A$2:$B$31,2,FALSE)</f>
+        <v>14</v>
+      </c>
+      <c r="C7" s="4">
         <v>1496</v>
       </c>
-      <c r="C7" s="66">
+      <c r="D7" s="66">
         <v>42981</v>
       </c>
-      <c r="D7" s="67">
+      <c r="E7" s="67">
         <v>0.64583333333333337</v>
       </c>
-      <c r="E7" s="68">
+      <c r="F7" s="68">
         <v>0</v>
       </c>
-      <c r="F7" s="68">
+      <c r="G7" s="68">
         <v>0.1</v>
       </c>
-      <c r="G7" s="4">
+      <c r="H7" s="4">
         <v>1631</v>
       </c>
-      <c r="H7" s="69">
+      <c r="I7" s="69">
         <f t="shared" si="0"/>
         <v>54.366666666666667</v>
       </c>
-      <c r="I7" s="77" t="s">
+      <c r="J7" s="77" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="11">
         <v>7</v>
       </c>
       <c r="B8" s="4">
+        <f>VLOOKUP(A8,'Order Chrono-Riviere'!$A$2:$B$31,2,FALSE)</f>
+        <v>20</v>
+      </c>
+      <c r="C8" s="4">
         <v>1527</v>
       </c>
-      <c r="C8" s="66">
+      <c r="D8" s="66">
         <v>42982</v>
       </c>
-      <c r="D8" s="67">
+      <c r="E8" s="67">
         <v>0.41666666666666669</v>
       </c>
-      <c r="E8" s="68">
-        <v>1</v>
-      </c>
       <c r="F8" s="68">
+        <v>1</v>
+      </c>
+      <c r="G8" s="68">
         <v>0.8</v>
       </c>
-      <c r="G8" s="4">
+      <c r="H8" s="4">
         <v>1652</v>
       </c>
-      <c r="H8" s="69">
+      <c r="I8" s="69">
         <f t="shared" si="0"/>
         <v>55.06666666666667</v>
       </c>
-      <c r="I8" s="77" t="s">
+      <c r="J8" s="77" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="11">
         <v>8</v>
       </c>
       <c r="B9" s="4">
+        <f>VLOOKUP(A9,'Order Chrono-Riviere'!$A$2:$B$31,2,FALSE)</f>
+        <v>21</v>
+      </c>
+      <c r="C9" s="4">
         <v>1559</v>
       </c>
-      <c r="C9" s="66">
+      <c r="D9" s="66">
         <v>42982</v>
       </c>
-      <c r="D9" s="67">
+      <c r="E9" s="67">
         <v>0.58333333333333337</v>
       </c>
-      <c r="E9" s="68">
+      <c r="F9" s="68">
         <v>0.9</v>
       </c>
-      <c r="F9" s="68">
+      <c r="G9" s="68">
         <v>0.95</v>
       </c>
-      <c r="G9" s="4">
+      <c r="H9" s="4">
         <v>1598</v>
       </c>
-      <c r="H9" s="69">
+      <c r="I9" s="69">
         <f t="shared" si="0"/>
         <v>53.266666666666666</v>
       </c>
-      <c r="I9" s="77" t="s">
+      <c r="J9" s="77" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="11">
         <v>9</v>
       </c>
       <c r="B10" s="4">
+        <f>VLOOKUP(A10,'Order Chrono-Riviere'!$A$2:$B$31,2,FALSE)</f>
+        <v>5</v>
+      </c>
+      <c r="C10" s="4">
         <v>1592</v>
       </c>
-      <c r="C10" s="66">
+      <c r="D10" s="66">
         <v>42983</v>
       </c>
-      <c r="D10" s="67">
+      <c r="E10" s="67">
         <v>0.4236111111111111</v>
       </c>
-      <c r="E10" s="68">
-        <v>1</v>
-      </c>
       <c r="F10" s="68">
         <v>1</v>
       </c>
-      <c r="G10" s="4">
+      <c r="G10" s="68">
+        <v>1</v>
+      </c>
+      <c r="H10" s="4">
         <v>1652</v>
       </c>
-      <c r="H10" s="69">
+      <c r="I10" s="69">
         <f t="shared" si="0"/>
         <v>55.06666666666667</v>
       </c>
-      <c r="I10" s="77" t="s">
+      <c r="J10" s="77" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="11">
         <v>10</v>
       </c>
       <c r="B11" s="4">
+        <f>VLOOKUP(A11,'Order Chrono-Riviere'!$A$2:$B$31,2,FALSE)</f>
+        <v>6</v>
+      </c>
+      <c r="C11" s="4">
         <v>1624</v>
       </c>
-      <c r="C11" s="66">
+      <c r="D11" s="66">
         <v>42983</v>
       </c>
-      <c r="D11" s="67">
+      <c r="E11" s="67">
         <v>0.55555555555555558</v>
       </c>
-      <c r="E11" s="68">
-        <v>1</v>
-      </c>
       <c r="F11" s="68">
         <v>1</v>
       </c>
-      <c r="G11" s="4">
+      <c r="G11" s="68">
+        <v>1</v>
+      </c>
+      <c r="H11" s="4">
         <v>1409</v>
       </c>
-      <c r="H11" s="69">
+      <c r="I11" s="69">
         <f t="shared" si="0"/>
         <v>46.966666666666669</v>
       </c>
-      <c r="I11" s="77" t="s">
+      <c r="J11" s="77" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="11">
         <v>11</v>
       </c>
       <c r="B12" s="4">
+        <f>VLOOKUP(A12,'Order Chrono-Riviere'!$A$2:$B$31,2,FALSE)</f>
+        <v>8</v>
+      </c>
+      <c r="C12" s="4">
         <v>1655</v>
       </c>
-      <c r="C12" s="66">
+      <c r="D12" s="66">
         <v>42983</v>
       </c>
-      <c r="D12" s="67">
+      <c r="E12" s="67">
         <v>0.68055555555555547</v>
       </c>
-      <c r="E12" s="68">
-        <v>1</v>
-      </c>
       <c r="F12" s="68">
         <v>1</v>
       </c>
-      <c r="G12" s="4" t="s">
+      <c r="G12" s="68">
+        <v>1</v>
+      </c>
+      <c r="H12" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="H12" s="69" t="s">
+      <c r="I12" s="69" t="s">
         <v>34</v>
       </c>
-      <c r="I12" s="77" t="s">
+      <c r="J12" s="77" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="11">
         <v>12</v>
       </c>
       <c r="B13" s="4">
+        <f>VLOOKUP(A13,'Order Chrono-Riviere'!$A$2:$B$31,2,FALSE)</f>
+        <v>10</v>
+      </c>
+      <c r="C13" s="4">
         <v>1686</v>
       </c>
-      <c r="C13" s="66">
+      <c r="D13" s="66">
         <v>42984</v>
       </c>
-      <c r="D13" s="67">
+      <c r="E13" s="67">
         <v>0.4236111111111111</v>
       </c>
-      <c r="E13" s="68">
+      <c r="F13" s="68">
         <v>0.9</v>
       </c>
-      <c r="F13" s="68">
-        <v>1</v>
-      </c>
-      <c r="G13" s="4">
+      <c r="G13" s="68">
+        <v>1</v>
+      </c>
+      <c r="H13" s="4">
         <v>1623</v>
       </c>
-      <c r="H13" s="69">
-        <f t="shared" ref="H13:H31" si="1">G13/30</f>
+      <c r="I13" s="69">
+        <f t="shared" ref="I13:I31" si="1">H13/30</f>
         <v>54.1</v>
       </c>
-      <c r="I13" s="77" t="s">
+      <c r="J13" s="77" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" s="11">
         <v>13</v>
       </c>
       <c r="B14" s="4">
+        <f>VLOOKUP(A14,'Order Chrono-Riviere'!$A$2:$B$31,2,FALSE)</f>
+        <v>15</v>
+      </c>
+      <c r="C14" s="4">
         <v>1730</v>
       </c>
-      <c r="C14" s="66">
+      <c r="D14" s="66">
         <v>42984</v>
       </c>
-      <c r="D14" s="67">
+      <c r="E14" s="67">
         <v>0.57430555555555551</v>
       </c>
-      <c r="E14" s="68">
-        <v>1</v>
-      </c>
       <c r="F14" s="68">
         <v>1</v>
       </c>
-      <c r="G14" s="4">
+      <c r="G14" s="68">
+        <v>1</v>
+      </c>
+      <c r="H14" s="4">
         <v>1523</v>
       </c>
-      <c r="H14" s="69">
+      <c r="I14" s="69">
         <f t="shared" si="1"/>
         <v>50.766666666666666</v>
       </c>
-      <c r="I14" s="77" t="s">
+      <c r="J14" s="77" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="11">
         <v>14</v>
       </c>
       <c r="B15" s="4">
+        <f>VLOOKUP(A15,'Order Chrono-Riviere'!$A$2:$B$31,2,FALSE)</f>
+        <v>16</v>
+      </c>
+      <c r="C15" s="4">
         <v>1761</v>
       </c>
-      <c r="C15" s="66">
+      <c r="D15" s="66">
         <v>42985</v>
       </c>
-      <c r="D15" s="67">
+      <c r="E15" s="67">
         <v>0.5625</v>
       </c>
-      <c r="E15" s="68">
-        <v>1</v>
-      </c>
       <c r="F15" s="68">
         <v>1</v>
       </c>
-      <c r="G15" s="4">
+      <c r="G15" s="68">
+        <v>1</v>
+      </c>
+      <c r="H15" s="4">
         <v>1652</v>
       </c>
-      <c r="H15" s="69">
+      <c r="I15" s="69">
         <f t="shared" si="1"/>
         <v>55.06666666666667</v>
       </c>
-      <c r="I15" s="77" t="s">
+      <c r="J15" s="77" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="11">
         <v>15</v>
       </c>
       <c r="B16" s="4">
+        <f>VLOOKUP(A16,'Order Chrono-Riviere'!$A$2:$B$31,2,FALSE)</f>
+        <v>11</v>
+      </c>
+      <c r="C16" s="4">
         <v>1793</v>
       </c>
-      <c r="C16" s="66">
+      <c r="D16" s="66">
         <v>42986</v>
       </c>
-      <c r="D16" s="67">
+      <c r="E16" s="67">
         <v>0.34027777777777773</v>
       </c>
-      <c r="E16" s="68">
+      <c r="F16" s="68">
         <v>0.2</v>
       </c>
-      <c r="F16" s="68">
-        <v>1</v>
-      </c>
-      <c r="G16" s="4">
+      <c r="G16" s="68">
+        <v>1</v>
+      </c>
+      <c r="H16" s="4">
         <v>1562</v>
       </c>
-      <c r="H16" s="69">
+      <c r="I16" s="69">
         <f t="shared" si="1"/>
         <v>52.06666666666667</v>
       </c>
-      <c r="I16" s="77" t="s">
+      <c r="J16" s="77" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="11">
         <v>16</v>
       </c>
       <c r="B17" s="4">
+        <f>VLOOKUP(A17,'Order Chrono-Riviere'!$A$2:$B$31,2,FALSE)</f>
+        <v>23</v>
+      </c>
+      <c r="C17" s="4">
         <v>1824</v>
       </c>
-      <c r="C17" s="66">
+      <c r="D17" s="66">
         <v>42986</v>
       </c>
-      <c r="D17" s="67">
+      <c r="E17" s="67">
         <v>0.46527777777777773</v>
       </c>
-      <c r="E17" s="68">
-        <v>1</v>
-      </c>
       <c r="F17" s="68">
         <v>1</v>
       </c>
-      <c r="G17" s="4">
+      <c r="G17" s="68">
+        <v>1</v>
+      </c>
+      <c r="H17" s="4">
         <v>1643</v>
       </c>
-      <c r="H17" s="69">
+      <c r="I17" s="69">
         <f t="shared" si="1"/>
         <v>54.766666666666666</v>
       </c>
-      <c r="I17" s="77" t="s">
+      <c r="J17" s="77" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="11">
         <v>17</v>
       </c>
       <c r="B18" s="4">
+        <f>VLOOKUP(A18,'Order Chrono-Riviere'!$A$2:$B$31,2,FALSE)</f>
+        <v>25</v>
+      </c>
+      <c r="C18" s="4">
         <v>1855</v>
       </c>
-      <c r="C18" s="66">
+      <c r="D18" s="66">
         <v>42986</v>
       </c>
-      <c r="D18" s="67">
+      <c r="E18" s="67">
         <v>0.59722222222222221</v>
       </c>
-      <c r="E18" s="68">
-        <v>1</v>
-      </c>
       <c r="F18" s="68">
         <v>1</v>
       </c>
-      <c r="G18" s="4">
+      <c r="G18" s="68">
+        <v>1</v>
+      </c>
+      <c r="H18" s="4">
         <v>1759</v>
       </c>
-      <c r="H18" s="69">
+      <c r="I18" s="69">
         <f t="shared" si="1"/>
         <v>58.633333333333333</v>
       </c>
-      <c r="I18" s="77" t="s">
+      <c r="J18" s="77" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="11">
         <v>18</v>
       </c>
       <c r="B19" s="4">
+        <f>VLOOKUP(A19,'Order Chrono-Riviere'!$A$2:$B$31,2,FALSE)</f>
+        <v>3</v>
+      </c>
+      <c r="C19" s="4">
         <v>1886</v>
       </c>
-      <c r="C19" s="66">
+      <c r="D19" s="66">
         <v>42989</v>
       </c>
-      <c r="D19" s="67">
+      <c r="E19" s="67">
         <v>0.3923611111111111</v>
-      </c>
-      <c r="E19" s="68">
-        <v>0</v>
       </c>
       <c r="F19" s="68">
         <v>0</v>
       </c>
-      <c r="G19" s="4">
+      <c r="G19" s="68">
+        <v>0</v>
+      </c>
+      <c r="H19" s="4">
         <v>1604</v>
       </c>
-      <c r="H19" s="69">
+      <c r="I19" s="69">
         <f t="shared" si="1"/>
         <v>53.466666666666669</v>
       </c>
-      <c r="I19" s="77" t="s">
+      <c r="J19" s="77" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="11">
         <v>19</v>
       </c>
       <c r="B20" s="4">
+        <f>VLOOKUP(A20,'Order Chrono-Riviere'!$A$2:$B$31,2,FALSE)</f>
+        <v>17</v>
+      </c>
+      <c r="C20" s="4">
         <v>1917</v>
       </c>
-      <c r="C20" s="66">
+      <c r="D20" s="66">
         <v>42989</v>
       </c>
-      <c r="D20" s="67">
+      <c r="E20" s="67">
         <v>0.55208333333333337</v>
-      </c>
-      <c r="E20" s="68">
-        <v>0</v>
       </c>
       <c r="F20" s="68">
         <v>0</v>
       </c>
-      <c r="G20" s="4">
+      <c r="G20" s="68">
+        <v>0</v>
+      </c>
+      <c r="H20" s="4">
         <v>1487</v>
       </c>
-      <c r="H20" s="69">
+      <c r="I20" s="69">
         <f t="shared" si="1"/>
         <v>49.56666666666667</v>
       </c>
-      <c r="I20" s="77" t="s">
+      <c r="J20" s="77" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="11">
         <v>20</v>
       </c>
       <c r="B21" s="4">
+        <f>VLOOKUP(A21,'Order Chrono-Riviere'!$A$2:$B$31,2,FALSE)</f>
+        <v>27</v>
+      </c>
+      <c r="C21" s="4">
         <v>1949</v>
       </c>
-      <c r="C21" s="66">
+      <c r="D21" s="66">
         <v>42990</v>
       </c>
-      <c r="D21" s="67">
+      <c r="E21" s="67">
         <v>0.36805555555555558</v>
-      </c>
-      <c r="E21" s="68">
-        <v>0</v>
       </c>
       <c r="F21" s="68">
         <v>0</v>
       </c>
-      <c r="G21" s="4">
+      <c r="G21" s="68">
+        <v>0</v>
+      </c>
+      <c r="H21" s="4">
         <v>1635</v>
       </c>
-      <c r="H21" s="69">
+      <c r="I21" s="69">
         <f t="shared" si="1"/>
         <v>54.5</v>
       </c>
-      <c r="I21" s="77" t="s">
+      <c r="J21" s="77" t="s">
         <v>111</v>
       </c>
-      <c r="J21" t="s">
+      <c r="K21" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="11">
         <v>21</v>
       </c>
       <c r="B22" s="4">
+        <f>VLOOKUP(A22,'Order Chrono-Riviere'!$A$2:$B$31,2,FALSE)</f>
+        <v>28</v>
+      </c>
+      <c r="C22" s="4">
         <v>1980</v>
       </c>
-      <c r="C22" s="66">
+      <c r="D22" s="66">
         <v>42990</v>
       </c>
-      <c r="D22" s="67">
+      <c r="E22" s="67">
         <v>0.54513888888888895</v>
       </c>
-      <c r="E22" s="68">
+      <c r="F22" s="68">
         <v>0.2</v>
       </c>
-      <c r="F22" s="68">
+      <c r="G22" s="68">
         <v>0.5</v>
       </c>
-      <c r="G22" s="4">
+      <c r="H22" s="4">
         <v>1753</v>
       </c>
-      <c r="H22" s="69">
+      <c r="I22" s="69">
         <f t="shared" si="1"/>
         <v>58.43333333333333</v>
       </c>
-      <c r="I22" s="77" t="s">
+      <c r="J22" s="77" t="s">
         <v>110</v>
       </c>
-      <c r="J22" t="s">
+      <c r="K22" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="11">
         <v>22</v>
       </c>
       <c r="B23" s="4">
+        <f>VLOOKUP(A23,'Order Chrono-Riviere'!$A$2:$B$31,2,FALSE)</f>
+        <v>30</v>
+      </c>
+      <c r="C23" s="4">
         <v>11</v>
       </c>
-      <c r="C23" s="66">
+      <c r="D23" s="66">
         <v>42990</v>
       </c>
-      <c r="D23" s="67">
+      <c r="E23" s="67">
         <v>0.62847222222222221</v>
       </c>
-      <c r="E23" s="68">
+      <c r="F23" s="68">
         <v>0.9</v>
       </c>
-      <c r="F23" s="68">
-        <v>1</v>
-      </c>
-      <c r="G23" s="4">
+      <c r="G23" s="68">
+        <v>1</v>
+      </c>
+      <c r="H23" s="4">
         <v>1662</v>
       </c>
-      <c r="H23" s="69">
+      <c r="I23" s="69">
         <f t="shared" si="1"/>
         <v>55.4</v>
       </c>
-      <c r="I23" s="77" t="s">
+      <c r="J23" s="77" t="s">
         <v>112</v>
       </c>
-      <c r="J23" t="s">
+      <c r="K23" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="11">
         <v>23</v>
       </c>
       <c r="B24" s="4">
+        <f>VLOOKUP(A24,'Order Chrono-Riviere'!$A$2:$B$31,2,FALSE)</f>
+        <v>7</v>
+      </c>
+      <c r="C24" s="4">
         <v>43</v>
       </c>
-      <c r="C24" s="66">
+      <c r="D24" s="66">
         <v>42991</v>
       </c>
-      <c r="D24" s="67">
+      <c r="E24" s="67">
         <v>0.47916666666666669</v>
       </c>
-      <c r="E24" s="68">
+      <c r="F24" s="68">
         <v>0.1</v>
       </c>
-      <c r="F24" s="68">
+      <c r="G24" s="68">
         <v>0</v>
       </c>
-      <c r="G24" s="4">
+      <c r="H24" s="4">
         <v>1647</v>
       </c>
-      <c r="H24" s="69">
+      <c r="I24" s="69">
         <f t="shared" si="1"/>
         <v>54.9</v>
       </c>
-      <c r="I24" s="77" t="s">
+      <c r="J24" s="77" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="11">
         <v>24</v>
       </c>
       <c r="B25" s="4">
+        <f>VLOOKUP(A25,'Order Chrono-Riviere'!$A$2:$B$31,2,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="C25" s="4">
         <v>74</v>
       </c>
-      <c r="C25" s="66">
+      <c r="D25" s="66">
         <v>42991</v>
       </c>
-      <c r="D25" s="67">
+      <c r="E25" s="67">
         <v>0.62847222222222221</v>
-      </c>
-      <c r="E25" s="68">
-        <v>0</v>
       </c>
       <c r="F25" s="68">
         <v>0</v>
       </c>
-      <c r="G25" s="4">
+      <c r="G25" s="68">
+        <v>0</v>
+      </c>
+      <c r="H25" s="4">
         <v>1622</v>
       </c>
-      <c r="H25" s="69">
+      <c r="I25" s="69">
         <f t="shared" si="1"/>
         <v>54.06666666666667</v>
       </c>
-      <c r="I25" s="77" t="s">
+      <c r="J25" s="77" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="11">
         <v>25</v>
       </c>
       <c r="B26" s="4">
+        <f>VLOOKUP(A26,'Order Chrono-Riviere'!$A$2:$B$31,2,FALSE)</f>
+        <v>22</v>
+      </c>
+      <c r="C26" s="4">
         <v>105</v>
       </c>
-      <c r="C26" s="66">
+      <c r="D26" s="66">
         <v>42992</v>
       </c>
-      <c r="D26" s="67">
+      <c r="E26" s="67">
         <v>0.43263888888888885</v>
-      </c>
-      <c r="E26" s="68">
-        <v>0</v>
       </c>
       <c r="F26" s="68">
         <v>0</v>
       </c>
-      <c r="G26" s="4">
+      <c r="G26" s="68">
+        <v>0</v>
+      </c>
+      <c r="H26" s="4">
         <v>1637</v>
       </c>
-      <c r="H26" s="69">
+      <c r="I26" s="69">
         <f t="shared" si="1"/>
         <v>54.56666666666667</v>
       </c>
-      <c r="I26" s="77" t="s">
+      <c r="J26" s="77" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="11">
         <v>26</v>
       </c>
       <c r="B27" s="4">
+        <f>VLOOKUP(A27,'Order Chrono-Riviere'!$A$2:$B$31,2,FALSE)</f>
+        <v>24</v>
+      </c>
+      <c r="C27" s="4">
         <v>136</v>
       </c>
-      <c r="C27" s="66">
+      <c r="D27" s="66">
         <v>42992</v>
       </c>
-      <c r="D27" s="67">
+      <c r="E27" s="67">
         <v>0.55763888888888891</v>
-      </c>
-      <c r="E27" s="68">
-        <v>0</v>
       </c>
       <c r="F27" s="68">
         <v>0</v>
       </c>
-      <c r="G27" s="4">
+      <c r="G27" s="68">
+        <v>0</v>
+      </c>
+      <c r="H27" s="4">
         <v>1601</v>
       </c>
-      <c r="H27" s="69">
+      <c r="I27" s="69">
         <f t="shared" si="1"/>
         <v>53.366666666666667</v>
       </c>
-      <c r="I27" s="77" t="s">
+      <c r="J27" s="77" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="11">
         <v>27</v>
       </c>
       <c r="B28" s="4">
+        <f>VLOOKUP(A28,'Order Chrono-Riviere'!$A$2:$B$31,2,FALSE)</f>
+        <v>26</v>
+      </c>
+      <c r="C28" s="4">
         <v>160</v>
       </c>
-      <c r="C28" s="66">
+      <c r="D28" s="66">
         <v>42993</v>
       </c>
-      <c r="D28" s="67">
+      <c r="E28" s="67">
         <v>0.45555555555555555</v>
-      </c>
-      <c r="E28" s="68">
-        <v>0</v>
       </c>
       <c r="F28" s="68">
         <v>0</v>
       </c>
-      <c r="G28" s="4">
+      <c r="G28" s="68">
+        <v>0</v>
+      </c>
+      <c r="H28" s="4">
         <v>1556</v>
       </c>
-      <c r="H28" s="69">
+      <c r="I28" s="69">
         <f t="shared" si="1"/>
         <v>51.866666666666667</v>
       </c>
-      <c r="I28" s="77" t="s">
+      <c r="J28" s="77" t="s">
         <v>139</v>
       </c>
-      <c r="J28" t="s">
+      <c r="K28" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="11">
         <v>28</v>
       </c>
       <c r="B29" s="4">
+        <f>VLOOKUP(A29,'Order Chrono-Riviere'!$A$2:$B$31,2,FALSE)</f>
+        <v>29</v>
+      </c>
+      <c r="C29" s="4">
         <v>191</v>
       </c>
-      <c r="C29" s="66">
+      <c r="D29" s="66">
         <v>42993</v>
       </c>
-      <c r="D29" s="67">
+      <c r="E29" s="67">
         <v>0.625</v>
-      </c>
-      <c r="E29" s="68">
-        <v>0</v>
       </c>
       <c r="F29" s="68">
         <v>0</v>
       </c>
-      <c r="G29" s="4">
+      <c r="G29" s="68">
+        <v>0</v>
+      </c>
+      <c r="H29" s="4">
         <v>1607</v>
       </c>
-      <c r="H29" s="69">
+      <c r="I29" s="69">
         <f t="shared" si="1"/>
         <v>53.56666666666667</v>
       </c>
-      <c r="I29" s="77" t="s">
+      <c r="J29" s="77" t="s">
         <v>131</v>
       </c>
-      <c r="J29" t="s">
+      <c r="K29" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="11">
         <v>29</v>
       </c>
       <c r="B30" s="4">
+        <f>VLOOKUP(A30,'Order Chrono-Riviere'!$A$2:$B$31,2,FALSE)</f>
+        <v>2</v>
+      </c>
+      <c r="C30" s="4">
         <v>222</v>
       </c>
-      <c r="C30" s="66">
+      <c r="D30" s="66">
         <v>42994</v>
       </c>
-      <c r="D30" s="67">
+      <c r="E30" s="67">
         <v>0.4236111111111111</v>
       </c>
-      <c r="E30" s="68">
+      <c r="F30" s="68">
         <v>0.1</v>
       </c>
-      <c r="F30" s="68">
-        <v>1</v>
-      </c>
-      <c r="G30" s="4">
+      <c r="G30" s="68">
+        <v>1</v>
+      </c>
+      <c r="H30" s="4">
         <v>1723</v>
       </c>
-      <c r="H30" s="69">
+      <c r="I30" s="69">
         <f t="shared" si="1"/>
         <v>57.43333333333333</v>
       </c>
-      <c r="I30" s="77" t="s">
+      <c r="J30" s="77" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="12">
         <v>30</v>
       </c>
       <c r="B31" s="21">
+        <f>VLOOKUP(A31,'Order Chrono-Riviere'!$A$2:$B$31,2,FALSE)</f>
+        <v>4</v>
+      </c>
+      <c r="C31" s="21">
         <v>253</v>
       </c>
-      <c r="C31" s="82">
+      <c r="D31" s="82">
         <v>42994</v>
       </c>
-      <c r="D31" s="83">
+      <c r="E31" s="83">
         <v>0.625</v>
       </c>
-      <c r="E31" s="78">
-        <v>1</v>
-      </c>
       <c r="F31" s="78">
         <v>1</v>
       </c>
-      <c r="G31" s="21">
+      <c r="G31" s="78">
+        <v>1</v>
+      </c>
+      <c r="H31" s="21">
         <v>1710</v>
       </c>
-      <c r="H31" s="84">
+      <c r="I31" s="84">
         <f t="shared" si="1"/>
         <v>57</v>
       </c>
-      <c r="I31" s="79" t="s">
+      <c r="J31" s="79" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="E32" s="5"/>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="F32" s="5"/>
-      <c r="H32" s="7"/>
-    </row>
-    <row r="33" spans="5:8" x14ac:dyDescent="0.2">
-      <c r="E33" s="5"/>
+      <c r="G32" s="5"/>
+      <c r="I32" s="7"/>
+    </row>
+    <row r="33" spans="6:9" x14ac:dyDescent="0.2">
       <c r="F33" s="5"/>
-      <c r="H33" s="7"/>
-    </row>
-    <row r="34" spans="5:8" x14ac:dyDescent="0.2">
-      <c r="E34" s="5"/>
+      <c r="G33" s="5"/>
+      <c r="I33" s="7"/>
+    </row>
+    <row r="34" spans="6:9" x14ac:dyDescent="0.2">
       <c r="F34" s="5"/>
-    </row>
-    <row r="35" spans="5:8" x14ac:dyDescent="0.2">
-      <c r="E35" s="5"/>
+      <c r="G34" s="5"/>
+    </row>
+    <row r="35" spans="6:9" x14ac:dyDescent="0.2">
       <c r="F35" s="5"/>
-    </row>
-    <row r="36" spans="5:8" x14ac:dyDescent="0.2">
-      <c r="E36" s="5"/>
+      <c r="G35" s="5"/>
+    </row>
+    <row r="36" spans="6:9" x14ac:dyDescent="0.2">
       <c r="F36" s="5"/>
-    </row>
-    <row r="37" spans="5:8" x14ac:dyDescent="0.2">
-      <c r="E37" s="5"/>
+      <c r="G36" s="5"/>
+    </row>
+    <row r="37" spans="6:9" x14ac:dyDescent="0.2">
       <c r="F37" s="5"/>
+      <c r="G37" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="K1:L1"/>
-    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="L3:M3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -64700,7 +64830,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{006E4F1A-9B48-E244-9465-9B82A093CBC9}">
   <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A15" workbookViewId="0">
       <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>

</xml_diff>